<commit_message>
:pencil2: | Mise à jour du journal de travail
</commit_message>
<xml_diff>
--- a/Documentation/Personnelle/Monteiro Rui - Journaux - ProjetWeb.xlsx
+++ b/Documentation/Personnelle/Monteiro Rui - Journaux - ProjetWeb.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="599" uniqueCount="136">
   <si>
     <t>JOURNAL DE TRAVAIL</t>
   </si>
@@ -766,6 +766,22 @@
   </si>
   <si>
     <t>1. Mise à jour du journal de travail</t>
+  </si>
+  <si>
+    <t>Réparation de la fonction de création d'annonces</t>
+  </si>
+  <si>
+    <t>1. Correction des erreures leur de l'enregistrement d'annonce</t>
+  </si>
+  <si>
+    <t>Fonctions et affichage d'une page Admin pour les annonces</t>
+  </si>
+  <si>
+    <t>1. Création des fonction pour l'effacement d'une annonce 
+2. Réalisation d'une page Admin pour voir toutes les annonces</t>
+  </si>
+  <si>
+    <t>Réalisation du journal de travail pour les jours précedents</t>
   </si>
 </sst>
 </file>
@@ -1544,8 +1560,8 @@
   </sheetPr>
   <dimension ref="A1:O396"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="N62" sqref="N62"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="G65" sqref="G65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1684,11 +1700,11 @@
       </c>
       <c r="C6" s="28">
         <f>SUM(I33:I396)</f>
-        <v>1.4861111111111103</v>
+        <v>1.0972222222222212</v>
       </c>
       <c r="D6" s="28">
         <f>B6+C6</f>
-        <v>2.7270833333333329</v>
+        <v>2.3381944444444436</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="2">
@@ -3438,78 +3454,100 @@
       </c>
       <c r="O57" s="1"/>
     </row>
-    <row r="58" spans="1:15" ht="13.5" thickBot="1">
+    <row r="58" spans="1:15" ht="26.25" thickBot="1">
       <c r="A58" s="1"/>
       <c r="B58" s="21"/>
       <c r="C58" s="21"/>
       <c r="D58" s="21"/>
       <c r="E58" s="1"/>
-      <c r="F58" s="2"/>
+      <c r="F58" s="2">
+        <v>44719</v>
+      </c>
       <c r="G58" s="3">
-        <v>0</v>
+        <v>0.5625</v>
       </c>
       <c r="H58" s="3">
-        <v>0</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="I58" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.10416666666666663</v>
       </c>
       <c r="J58" s="15"/>
-      <c r="K58" s="15"/>
-      <c r="L58" s="6"/>
+      <c r="K58" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="L58" s="6" t="s">
+        <v>131</v>
+      </c>
       <c r="M58" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="N58" s="8"/>
+      <c r="N58" s="8" t="s">
+        <v>132</v>
+      </c>
       <c r="O58" s="1"/>
     </row>
-    <row r="59" spans="1:15" ht="13.5" thickBot="1">
+    <row r="59" spans="1:15" ht="26.25" thickBot="1">
       <c r="A59" s="1"/>
       <c r="B59" s="21"/>
       <c r="C59" s="21"/>
       <c r="D59" s="21"/>
       <c r="E59" s="1"/>
-      <c r="F59" s="2"/>
+      <c r="F59" s="2">
+        <v>44721</v>
+      </c>
       <c r="G59" s="3">
-        <v>0</v>
+        <v>0.59722222222222221</v>
       </c>
       <c r="H59" s="3">
-        <v>0</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="I59" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>6.944444444444442E-2</v>
       </c>
       <c r="J59" s="15"/>
-      <c r="K59" s="15"/>
-      <c r="L59" s="6"/>
+      <c r="K59" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="L59" s="6" t="s">
+        <v>133</v>
+      </c>
       <c r="M59" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="N59" s="8"/>
+      <c r="N59" s="8" t="s">
+        <v>134</v>
+      </c>
       <c r="O59" s="1"/>
     </row>
-    <row r="60" spans="1:15" ht="13.5" thickBot="1">
+    <row r="60" spans="1:15" ht="26.25" thickBot="1">
       <c r="A60" s="1"/>
       <c r="B60" s="21"/>
       <c r="C60" s="21"/>
       <c r="D60" s="21"/>
       <c r="E60" s="1"/>
-      <c r="F60" s="2"/>
+      <c r="F60" s="2">
+        <v>44722</v>
+      </c>
       <c r="G60" s="3">
-        <v>0</v>
+        <v>0.5625</v>
       </c>
       <c r="H60" s="3">
-        <v>0</v>
+        <v>0.56944444444444442</v>
       </c>
       <c r="I60" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>6.9444444444444198E-3</v>
       </c>
       <c r="J60" s="15"/>
-      <c r="K60" s="15"/>
-      <c r="L60" s="6"/>
+      <c r="K60" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="L60" s="6" t="s">
+        <v>135</v>
+      </c>
       <c r="M60" s="23" t="s">
         <v>13</v>
       </c>
@@ -3522,16 +3560,18 @@
       <c r="C61" s="21"/>
       <c r="D61" s="21"/>
       <c r="E61" s="1"/>
-      <c r="F61" s="2"/>
+      <c r="F61" s="2">
+        <v>44722</v>
+      </c>
       <c r="G61" s="3">
-        <v>0</v>
+        <v>0.56944444444444442</v>
       </c>
       <c r="H61" s="3">
         <v>0</v>
       </c>
       <c r="I61" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-0.56944444444444442</v>
       </c>
       <c r="J61" s="15"/>
       <c r="K61" s="15"/>

</xml_diff>

<commit_message>
:pencil2: | Mise à jour de la documentation
</commit_message>
<xml_diff>
--- a/Documentation/Personnelle/Monteiro Rui - Journaux - ProjetWeb.xlsx
+++ b/Documentation/Personnelle/Monteiro Rui - Journaux - ProjetWeb.xlsx
@@ -1,27 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rui-Miguel.MONTEIRO\Desktop\Projects\CPNV\Anubis-V2\Documentation\Personnelle\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\Pojetos\CPNV\Anubis-V2\Documentation\Personnelle\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00B33360-057C-44D5-BDDC-29D66905E2FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8205"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Travail" sheetId="1" r:id="rId1"/>
     <sheet name="Bord" sheetId="2" r:id="rId2"/>
     <sheet name="⚙️ Settings" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="599" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="139">
   <si>
     <t>JOURNAL DE TRAVAIL</t>
   </si>
@@ -783,17 +796,28 @@
   <si>
     <t>Réalisation du journal de travail pour les jours précedents</t>
   </si>
+  <si>
+    <t>Affichage des annonces</t>
+  </si>
+  <si>
+    <t>1. Tentative de correction de l'affichage des annonces</t>
+  </si>
+  <si>
+    <t>1. Correction de l'affichage des annonces, une div CSS importante pour l'affichage par ligne n'avais pas été copiée lors du changement donc j'ai du retrouver le template pour tou reverifier et faire tous les tests
+2. Mise en forme de l'image pour l'affichage 
+3. Changement du script SQL car le champ pour l'image avait une limite trop petite</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="yyyy/mm/dd"/>
     <numFmt numFmtId="165" formatCode="dd&quot;/&quot;mm&quot;/&quot;yyyy"/>
     <numFmt numFmtId="166" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1552,7 +1576,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor rgb="FF00FFFF"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -1561,10 +1585,10 @@
   <dimension ref="A1:O396"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="G65" sqref="G65"/>
+      <selection activeCell="D62" sqref="D62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="0.85546875" customWidth="1"/>
     <col min="2" max="2" width="12.5703125" customWidth="1"/>
@@ -1579,7 +1603,7 @@
     <col min="16" max="16384" width="12.5703125" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="6" customHeight="1" thickBot="1">
+    <row r="1" spans="1:15" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -1596,7 +1620,7 @@
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
     </row>
-    <row r="2" spans="1:15" ht="27" customHeight="1" thickTop="1">
+    <row r="2" spans="1:15" ht="27" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="29" t="s">
         <v>75</v>
@@ -1617,7 +1641,7 @@
       <c r="N2" s="31"/>
       <c r="O2" s="1"/>
     </row>
-    <row r="3" spans="1:15" ht="27" customHeight="1" thickBot="1">
+    <row r="3" spans="1:15" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="32"/>
       <c r="C3" s="33"/>
@@ -1634,7 +1658,7 @@
       <c r="N3" s="34"/>
       <c r="O3" s="1"/>
     </row>
-    <row r="4" spans="1:15" ht="19.5" customHeight="1" thickTop="1">
+    <row r="4" spans="1:15" ht="19.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
       <c r="B4" s="35" t="s">
         <v>107</v>
@@ -1675,7 +1699,7 @@
       </c>
       <c r="O4" s="1"/>
     </row>
-    <row r="5" spans="1:15" ht="19.5" customHeight="1" thickBot="1">
+    <row r="5" spans="1:15" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="36"/>
       <c r="C5" s="36"/>
@@ -1692,7 +1716,7 @@
       <c r="N5" s="44"/>
       <c r="O5" s="1"/>
     </row>
-    <row r="6" spans="1:15" ht="78" thickTop="1" thickBot="1">
+    <row r="6" spans="1:15" ht="78" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="27">
         <f>SUM(I6:I30)</f>
@@ -1700,11 +1724,11 @@
       </c>
       <c r="C6" s="28">
         <f>SUM(I33:I396)</f>
-        <v>1.0972222222222212</v>
+        <v>1.826388888888888</v>
       </c>
       <c r="D6" s="28">
         <f>B6+C6</f>
-        <v>2.3381944444444436</v>
+        <v>3.0673611111111105</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="2">
@@ -1737,7 +1761,7 @@
       </c>
       <c r="O6" s="1"/>
     </row>
-    <row r="7" spans="1:15" ht="39.75" thickTop="1" thickBot="1">
+    <row r="7" spans="1:15" ht="39.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="22"/>
       <c r="C7" s="22"/>
@@ -1773,7 +1797,7 @@
       </c>
       <c r="O7" s="1"/>
     </row>
-    <row r="8" spans="1:15" ht="39" thickBot="1">
+    <row r="8" spans="1:15" ht="39" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="21"/>
       <c r="C8" s="21"/>
@@ -1809,7 +1833,7 @@
       </c>
       <c r="O8" s="1"/>
     </row>
-    <row r="9" spans="1:15" ht="25.5">
+    <row r="9" spans="1:15" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
       <c r="B9" s="21"/>
       <c r="C9" s="21"/>
@@ -1845,7 +1869,7 @@
       </c>
       <c r="O9" s="1"/>
     </row>
-    <row r="10" spans="1:15" ht="12.75">
+    <row r="10" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
       <c r="B10" s="21"/>
       <c r="C10" s="21"/>
@@ -1881,7 +1905,7 @@
       </c>
       <c r="O10" s="1"/>
     </row>
-    <row r="11" spans="1:15" ht="12.75">
+    <row r="11" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="9"/>
       <c r="B11" s="21"/>
       <c r="C11" s="21"/>
@@ -1917,7 +1941,7 @@
       </c>
       <c r="O11" s="1"/>
     </row>
-    <row r="12" spans="1:15" ht="25.5">
+    <row r="12" spans="1:15" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
       <c r="B12" s="21"/>
       <c r="C12" s="21"/>
@@ -1953,7 +1977,7 @@
       </c>
       <c r="O12" s="1"/>
     </row>
-    <row r="13" spans="1:15" ht="12.75">
+    <row r="13" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
       <c r="B13" s="21"/>
       <c r="C13" s="21"/>
@@ -1989,7 +2013,7 @@
       </c>
       <c r="O13" s="1"/>
     </row>
-    <row r="14" spans="1:15" ht="25.5">
+    <row r="14" spans="1:15" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
       <c r="B14" s="21"/>
       <c r="C14" s="21"/>
@@ -2025,7 +2049,7 @@
       </c>
       <c r="O14" s="1"/>
     </row>
-    <row r="15" spans="1:15" ht="51">
+    <row r="15" spans="1:15" ht="51" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
       <c r="B15" s="21"/>
       <c r="C15" s="21"/>
@@ -2061,7 +2085,7 @@
       </c>
       <c r="O15" s="1"/>
     </row>
-    <row r="16" spans="1:15" ht="25.5">
+    <row r="16" spans="1:15" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
       <c r="B16" s="21"/>
       <c r="C16" s="21"/>
@@ -2097,7 +2121,7 @@
       </c>
       <c r="O16" s="1"/>
     </row>
-    <row r="17" spans="1:15" ht="12.75">
+    <row r="17" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
       <c r="B17" s="21"/>
       <c r="C17" s="21"/>
@@ -2133,7 +2157,7 @@
       </c>
       <c r="O17" s="1"/>
     </row>
-    <row r="18" spans="1:15" ht="25.5">
+    <row r="18" spans="1:15" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
       <c r="B18" s="21"/>
       <c r="C18" s="21"/>
@@ -2169,7 +2193,7 @@
       </c>
       <c r="O18" s="1"/>
     </row>
-    <row r="19" spans="1:15" ht="12.75">
+    <row r="19" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19" s="1"/>
       <c r="B19" s="21"/>
       <c r="C19" s="21"/>
@@ -2203,7 +2227,7 @@
       </c>
       <c r="O19" s="1"/>
     </row>
-    <row r="20" spans="1:15" ht="12.75">
+    <row r="20" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>
       <c r="B20" s="21"/>
       <c r="C20" s="21"/>
@@ -2230,7 +2254,7 @@
       <c r="N20" s="14"/>
       <c r="O20" s="1"/>
     </row>
-    <row r="21" spans="1:15" ht="12.75">
+    <row r="21" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
       <c r="B21" s="21"/>
       <c r="C21" s="21"/>
@@ -2264,7 +2288,7 @@
       </c>
       <c r="O21" s="1"/>
     </row>
-    <row r="22" spans="1:15" ht="12.75">
+    <row r="22" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
       <c r="B22" s="21"/>
       <c r="C22" s="21"/>
@@ -2298,7 +2322,7 @@
       </c>
       <c r="O22" s="1"/>
     </row>
-    <row r="23" spans="1:15" ht="12.75">
+    <row r="23" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="1"/>
       <c r="B23" s="21"/>
       <c r="C23" s="21"/>
@@ -2332,7 +2356,7 @@
       </c>
       <c r="O23" s="1"/>
     </row>
-    <row r="24" spans="1:15" ht="12.75">
+    <row r="24" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="1"/>
       <c r="B24" s="21"/>
       <c r="C24" s="21"/>
@@ -2366,7 +2390,7 @@
       </c>
       <c r="O24" s="1"/>
     </row>
-    <row r="25" spans="1:15" ht="38.25">
+    <row r="25" spans="1:15" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A25" s="1"/>
       <c r="B25" s="21"/>
       <c r="C25" s="21"/>
@@ -2400,7 +2424,7 @@
       </c>
       <c r="O25" s="1"/>
     </row>
-    <row r="26" spans="1:15" ht="25.5">
+    <row r="26" spans="1:15" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A26" s="1"/>
       <c r="B26" s="21"/>
       <c r="C26" s="21"/>
@@ -2434,7 +2458,7 @@
       </c>
       <c r="O26" s="1"/>
     </row>
-    <row r="27" spans="1:15" ht="25.5">
+    <row r="27" spans="1:15" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A27" s="1"/>
       <c r="B27" s="21"/>
       <c r="C27" s="21"/>
@@ -2468,7 +2492,7 @@
       </c>
       <c r="O27" s="1"/>
     </row>
-    <row r="28" spans="1:15" ht="12.75">
+    <row r="28" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="1"/>
       <c r="B28" s="21"/>
       <c r="C28" s="21"/>
@@ -2502,7 +2526,7 @@
       </c>
       <c r="O28" s="1"/>
     </row>
-    <row r="29" spans="1:15" ht="25.5">
+    <row r="29" spans="1:15" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A29" s="1"/>
       <c r="B29" s="21"/>
       <c r="C29" s="21"/>
@@ -2536,7 +2560,7 @@
       </c>
       <c r="O29" s="1"/>
     </row>
-    <row r="30" spans="1:15" ht="77.25" thickBot="1">
+    <row r="30" spans="1:15" ht="77.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="21"/>
       <c r="C30" s="21"/>
@@ -2570,7 +2594,7 @@
       </c>
       <c r="O30" s="1"/>
     </row>
-    <row r="31" spans="1:15" ht="15" customHeight="1" thickTop="1">
+    <row r="31" spans="1:15" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A31" s="1"/>
       <c r="B31" s="21"/>
       <c r="C31" s="21"/>
@@ -2589,7 +2613,7 @@
       <c r="N31" s="39"/>
       <c r="O31" s="1"/>
     </row>
-    <row r="32" spans="1:15" ht="13.5" thickBot="1">
+    <row r="32" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="21"/>
       <c r="C32" s="21"/>
@@ -2606,7 +2630,7 @@
       <c r="N32" s="42"/>
       <c r="O32" s="1"/>
     </row>
-    <row r="33" spans="1:15" ht="27" thickTop="1" thickBot="1">
+    <row r="33" spans="1:15" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="21"/>
       <c r="C33" s="21"/>
@@ -2640,7 +2664,7 @@
       </c>
       <c r="O33" s="1"/>
     </row>
-    <row r="34" spans="1:15" ht="26.25" thickBot="1">
+    <row r="34" spans="1:15" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="21"/>
       <c r="C34" s="21"/>
@@ -2674,7 +2698,7 @@
       </c>
       <c r="O34" s="1"/>
     </row>
-    <row r="35" spans="1:15" ht="26.25" thickBot="1">
+    <row r="35" spans="1:15" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="21"/>
       <c r="C35" s="21"/>
@@ -2708,7 +2732,7 @@
       </c>
       <c r="O35" s="1"/>
     </row>
-    <row r="36" spans="1:15" ht="51.75" thickBot="1">
+    <row r="36" spans="1:15" ht="51.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="21"/>
       <c r="C36" s="21"/>
@@ -2742,7 +2766,7 @@
       </c>
       <c r="O36" s="1"/>
     </row>
-    <row r="37" spans="1:15" ht="26.25" thickBot="1">
+    <row r="37" spans="1:15" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="21"/>
       <c r="C37" s="21"/>
@@ -2776,7 +2800,7 @@
       </c>
       <c r="O37" s="1"/>
     </row>
-    <row r="38" spans="1:15" ht="13.5" thickBot="1">
+    <row r="38" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="21"/>
       <c r="C38" s="21"/>
@@ -2810,7 +2834,7 @@
       </c>
       <c r="O38" s="1"/>
     </row>
-    <row r="39" spans="1:15" ht="13.5" thickBot="1">
+    <row r="39" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="21"/>
       <c r="C39" s="21"/>
@@ -2844,7 +2868,7 @@
       </c>
       <c r="O39" s="1"/>
     </row>
-    <row r="40" spans="1:15" ht="13.5" thickBot="1">
+    <row r="40" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="21"/>
       <c r="C40" s="21"/>
@@ -2878,7 +2902,7 @@
       </c>
       <c r="O40" s="1"/>
     </row>
-    <row r="41" spans="1:15" ht="13.5" thickBot="1">
+    <row r="41" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="21"/>
       <c r="C41" s="21"/>
@@ -2912,7 +2936,7 @@
       </c>
       <c r="O41" s="1"/>
     </row>
-    <row r="42" spans="1:15" ht="13.5" thickBot="1">
+    <row r="42" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="21"/>
       <c r="C42" s="21"/>
@@ -2946,7 +2970,7 @@
       </c>
       <c r="O42" s="1"/>
     </row>
-    <row r="43" spans="1:15" ht="13.5" thickBot="1">
+    <row r="43" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="21"/>
       <c r="C43" s="21"/>
@@ -2980,7 +3004,7 @@
       </c>
       <c r="O43" s="1"/>
     </row>
-    <row r="44" spans="1:15" ht="13.5" thickBot="1">
+    <row r="44" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="21"/>
       <c r="C44" s="21"/>
@@ -3014,7 +3038,7 @@
       </c>
       <c r="O44" s="1"/>
     </row>
-    <row r="45" spans="1:15" ht="13.5" thickBot="1">
+    <row r="45" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="21"/>
       <c r="C45" s="21"/>
@@ -3048,7 +3072,7 @@
       </c>
       <c r="O45" s="1"/>
     </row>
-    <row r="46" spans="1:15" ht="77.25" thickBot="1">
+    <row r="46" spans="1:15" ht="77.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="21"/>
       <c r="C46" s="21"/>
@@ -3082,7 +3106,7 @@
       </c>
       <c r="O46" s="1"/>
     </row>
-    <row r="47" spans="1:15" ht="39" thickBot="1">
+    <row r="47" spans="1:15" ht="39" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="21"/>
       <c r="C47" s="21"/>
@@ -3116,7 +3140,7 @@
       </c>
       <c r="O47" s="1"/>
     </row>
-    <row r="48" spans="1:15" ht="26.25" thickBot="1">
+    <row r="48" spans="1:15" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" s="21"/>
       <c r="C48" s="21"/>
@@ -3150,7 +3174,7 @@
       </c>
       <c r="O48" s="1"/>
     </row>
-    <row r="49" spans="1:15" ht="13.5" thickBot="1">
+    <row r="49" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
       <c r="B49" s="21"/>
       <c r="C49" s="21"/>
@@ -3184,7 +3208,7 @@
       </c>
       <c r="O49" s="1"/>
     </row>
-    <row r="50" spans="1:15" ht="26.25" thickBot="1">
+    <row r="50" spans="1:15" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="B50" s="21"/>
       <c r="C50" s="21"/>
@@ -3218,7 +3242,7 @@
       </c>
       <c r="O50" s="1"/>
     </row>
-    <row r="51" spans="1:15" ht="13.5" thickBot="1">
+    <row r="51" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
       <c r="B51" s="21"/>
       <c r="C51" s="21"/>
@@ -3252,7 +3276,7 @@
       </c>
       <c r="O51" s="1"/>
     </row>
-    <row r="52" spans="1:15" ht="13.5" thickBot="1">
+    <row r="52" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
       <c r="B52" s="21"/>
       <c r="C52" s="21"/>
@@ -3286,7 +3310,7 @@
       </c>
       <c r="O52" s="1"/>
     </row>
-    <row r="53" spans="1:15" ht="13.5" thickBot="1">
+    <row r="53" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
       <c r="B53" s="21"/>
       <c r="C53" s="21"/>
@@ -3320,7 +3344,7 @@
       </c>
       <c r="O53" s="1"/>
     </row>
-    <row r="54" spans="1:15" ht="51.75" thickBot="1">
+    <row r="54" spans="1:15" ht="51.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
       <c r="B54" s="21"/>
       <c r="C54" s="21"/>
@@ -3354,7 +3378,7 @@
       </c>
       <c r="O54" s="1"/>
     </row>
-    <row r="55" spans="1:15" ht="26.25" thickBot="1">
+    <row r="55" spans="1:15" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
       <c r="B55" s="21"/>
       <c r="C55" s="21"/>
@@ -3386,7 +3410,7 @@
       <c r="N55" s="8"/>
       <c r="O55" s="1"/>
     </row>
-    <row r="56" spans="1:15" ht="51.75" thickBot="1">
+    <row r="56" spans="1:15" ht="51.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
       <c r="B56" s="21"/>
       <c r="C56" s="21"/>
@@ -3420,7 +3444,7 @@
       </c>
       <c r="O56" s="1"/>
     </row>
-    <row r="57" spans="1:15" ht="13.5" thickBot="1">
+    <row r="57" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
       <c r="B57" s="21"/>
       <c r="C57" s="21"/>
@@ -3454,7 +3478,7 @@
       </c>
       <c r="O57" s="1"/>
     </row>
-    <row r="58" spans="1:15" ht="26.25" thickBot="1">
+    <row r="58" spans="1:15" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
       <c r="B58" s="21"/>
       <c r="C58" s="21"/>
@@ -3488,7 +3512,7 @@
       </c>
       <c r="O58" s="1"/>
     </row>
-    <row r="59" spans="1:15" ht="26.25" thickBot="1">
+    <row r="59" spans="1:15" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
       <c r="B59" s="21"/>
       <c r="C59" s="21"/>
@@ -3522,7 +3546,7 @@
       </c>
       <c r="O59" s="1"/>
     </row>
-    <row r="60" spans="1:15" ht="26.25" thickBot="1">
+    <row r="60" spans="1:15" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
       <c r="B60" s="21"/>
       <c r="C60" s="21"/>
@@ -3554,7 +3578,7 @@
       <c r="N60" s="8"/>
       <c r="O60" s="1"/>
     </row>
-    <row r="61" spans="1:15" ht="13.5" thickBot="1">
+    <row r="61" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
       <c r="B61" s="21"/>
       <c r="C61" s="21"/>
@@ -3567,48 +3591,62 @@
         <v>0.56944444444444442</v>
       </c>
       <c r="H61" s="3">
-        <v>0</v>
+        <v>0.625</v>
       </c>
       <c r="I61" s="4">
         <f t="shared" si="2"/>
-        <v>-0.56944444444444442</v>
+        <v>5.555555555555558E-2</v>
       </c>
       <c r="J61" s="15"/>
-      <c r="K61" s="15"/>
-      <c r="L61" s="6"/>
+      <c r="K61" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="L61" s="6" t="s">
+        <v>136</v>
+      </c>
       <c r="M61" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="N61" s="8"/>
+      <c r="N61" s="8" t="s">
+        <v>137</v>
+      </c>
       <c r="O61" s="1"/>
     </row>
-    <row r="62" spans="1:15" ht="13.5" thickBot="1">
+    <row r="62" spans="1:15" ht="64.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
       <c r="B62" s="21"/>
       <c r="C62" s="21"/>
       <c r="D62" s="21"/>
       <c r="E62" s="1"/>
-      <c r="F62" s="2"/>
+      <c r="F62" s="2">
+        <v>44723</v>
+      </c>
       <c r="G62" s="3">
-        <v>0</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="H62" s="3">
-        <v>0</v>
+        <v>0.1875</v>
       </c>
       <c r="I62" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.10416666666666667</v>
       </c>
       <c r="J62" s="15"/>
-      <c r="K62" s="15"/>
-      <c r="L62" s="6"/>
+      <c r="K62" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="L62" s="6" t="s">
+        <v>136</v>
+      </c>
       <c r="M62" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="N62" s="8"/>
+      <c r="N62" s="8" t="s">
+        <v>138</v>
+      </c>
       <c r="O62" s="1"/>
     </row>
-    <row r="63" spans="1:15" ht="13.5" thickBot="1">
+    <row r="63" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
       <c r="B63" s="21"/>
       <c r="C63" s="21"/>
@@ -3634,7 +3672,7 @@
       <c r="N63" s="8"/>
       <c r="O63" s="1"/>
     </row>
-    <row r="64" spans="1:15" ht="13.5" thickBot="1">
+    <row r="64" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
       <c r="B64" s="21"/>
       <c r="C64" s="21"/>
@@ -3660,7 +3698,7 @@
       <c r="N64" s="8"/>
       <c r="O64" s="1"/>
     </row>
-    <row r="65" spans="1:15" ht="13.5" thickBot="1">
+    <row r="65" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
       <c r="B65" s="21"/>
       <c r="C65" s="21"/>
@@ -3686,7 +3724,7 @@
       <c r="N65" s="8"/>
       <c r="O65" s="1"/>
     </row>
-    <row r="66" spans="1:15" ht="13.5" thickBot="1">
+    <row r="66" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
       <c r="B66" s="21"/>
       <c r="C66" s="21"/>
@@ -3712,7 +3750,7 @@
       <c r="N66" s="8"/>
       <c r="O66" s="1"/>
     </row>
-    <row r="67" spans="1:15" ht="13.5" thickBot="1">
+    <row r="67" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
       <c r="B67" s="21"/>
       <c r="C67" s="21"/>
@@ -3738,7 +3776,7 @@
       <c r="N67" s="8"/>
       <c r="O67" s="1"/>
     </row>
-    <row r="68" spans="1:15" ht="13.5" thickBot="1">
+    <row r="68" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
       <c r="B68" s="21"/>
       <c r="C68" s="21"/>
@@ -3764,7 +3802,7 @@
       <c r="N68" s="8"/>
       <c r="O68" s="1"/>
     </row>
-    <row r="69" spans="1:15" ht="13.5" thickBot="1">
+    <row r="69" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
       <c r="B69" s="21"/>
       <c r="C69" s="21"/>
@@ -3790,7 +3828,7 @@
       <c r="N69" s="8"/>
       <c r="O69" s="1"/>
     </row>
-    <row r="70" spans="1:15" ht="13.5" thickBot="1">
+    <row r="70" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
       <c r="B70" s="21"/>
       <c r="C70" s="21"/>
@@ -3816,7 +3854,7 @@
       <c r="N70" s="8"/>
       <c r="O70" s="1"/>
     </row>
-    <row r="71" spans="1:15" ht="13.5" thickBot="1">
+    <row r="71" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
       <c r="B71" s="21"/>
       <c r="C71" s="21"/>
@@ -3842,7 +3880,7 @@
       <c r="N71" s="8"/>
       <c r="O71" s="1"/>
     </row>
-    <row r="72" spans="1:15" ht="13.5" thickBot="1">
+    <row r="72" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A72" s="1"/>
       <c r="B72" s="21"/>
       <c r="C72" s="21"/>
@@ -3868,7 +3906,7 @@
       <c r="N72" s="8"/>
       <c r="O72" s="1"/>
     </row>
-    <row r="73" spans="1:15" ht="13.5" thickBot="1">
+    <row r="73" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A73" s="1"/>
       <c r="B73" s="21"/>
       <c r="C73" s="21"/>
@@ -3894,7 +3932,7 @@
       <c r="N73" s="8"/>
       <c r="O73" s="1"/>
     </row>
-    <row r="74" spans="1:15" ht="13.5" thickBot="1">
+    <row r="74" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
       <c r="B74" s="21"/>
       <c r="C74" s="21"/>
@@ -3920,7 +3958,7 @@
       <c r="N74" s="8"/>
       <c r="O74" s="1"/>
     </row>
-    <row r="75" spans="1:15" ht="13.5" thickBot="1">
+    <row r="75" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
       <c r="B75" s="21"/>
       <c r="C75" s="21"/>
@@ -3946,7 +3984,7 @@
       <c r="N75" s="8"/>
       <c r="O75" s="1"/>
     </row>
-    <row r="76" spans="1:15" ht="13.5" thickBot="1">
+    <row r="76" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A76" s="1"/>
       <c r="B76" s="21"/>
       <c r="C76" s="21"/>
@@ -3972,7 +4010,7 @@
       <c r="N76" s="8"/>
       <c r="O76" s="1"/>
     </row>
-    <row r="77" spans="1:15" ht="13.5" thickBot="1">
+    <row r="77" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A77" s="1"/>
       <c r="B77" s="21"/>
       <c r="C77" s="21"/>
@@ -3998,7 +4036,7 @@
       <c r="N77" s="8"/>
       <c r="O77" s="1"/>
     </row>
-    <row r="78" spans="1:15" ht="13.5" thickBot="1">
+    <row r="78" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A78" s="1"/>
       <c r="B78" s="21"/>
       <c r="C78" s="21"/>
@@ -4024,7 +4062,7 @@
       <c r="N78" s="8"/>
       <c r="O78" s="1"/>
     </row>
-    <row r="79" spans="1:15" ht="13.5" thickBot="1">
+    <row r="79" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A79" s="1"/>
       <c r="B79" s="21"/>
       <c r="C79" s="21"/>
@@ -4050,7 +4088,7 @@
       <c r="N79" s="8"/>
       <c r="O79" s="1"/>
     </row>
-    <row r="80" spans="1:15" ht="13.5" thickBot="1">
+    <row r="80" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
       <c r="B80" s="21"/>
       <c r="C80" s="21"/>
@@ -4076,7 +4114,7 @@
       <c r="N80" s="8"/>
       <c r="O80" s="1"/>
     </row>
-    <row r="81" spans="1:15" ht="13.5" thickBot="1">
+    <row r="81" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A81" s="1"/>
       <c r="B81" s="21"/>
       <c r="C81" s="21"/>
@@ -4102,7 +4140,7 @@
       <c r="N81" s="8"/>
       <c r="O81" s="1"/>
     </row>
-    <row r="82" spans="1:15" ht="13.5" thickBot="1">
+    <row r="82" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A82" s="1"/>
       <c r="B82" s="21"/>
       <c r="C82" s="21"/>
@@ -4128,7 +4166,7 @@
       <c r="N82" s="8"/>
       <c r="O82" s="1"/>
     </row>
-    <row r="83" spans="1:15" ht="13.5" thickBot="1">
+    <row r="83" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A83" s="1"/>
       <c r="B83" s="21"/>
       <c r="C83" s="21"/>
@@ -4154,7 +4192,7 @@
       <c r="N83" s="8"/>
       <c r="O83" s="1"/>
     </row>
-    <row r="84" spans="1:15" ht="13.5" thickBot="1">
+    <row r="84" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A84" s="1"/>
       <c r="B84" s="21"/>
       <c r="C84" s="21"/>
@@ -4180,7 +4218,7 @@
       <c r="N84" s="8"/>
       <c r="O84" s="1"/>
     </row>
-    <row r="85" spans="1:15" ht="13.5" thickBot="1">
+    <row r="85" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A85" s="1"/>
       <c r="B85" s="21"/>
       <c r="C85" s="21"/>
@@ -4206,7 +4244,7 @@
       <c r="N85" s="8"/>
       <c r="O85" s="1"/>
     </row>
-    <row r="86" spans="1:15" ht="13.5" thickBot="1">
+    <row r="86" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A86" s="1"/>
       <c r="B86" s="21"/>
       <c r="C86" s="21"/>
@@ -4232,7 +4270,7 @@
       <c r="N86" s="8"/>
       <c r="O86" s="1"/>
     </row>
-    <row r="87" spans="1:15" ht="13.5" thickBot="1">
+    <row r="87" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A87" s="1"/>
       <c r="B87" s="21"/>
       <c r="C87" s="21"/>
@@ -4258,7 +4296,7 @@
       <c r="N87" s="8"/>
       <c r="O87" s="1"/>
     </row>
-    <row r="88" spans="1:15" ht="13.5" thickBot="1">
+    <row r="88" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A88" s="1"/>
       <c r="B88" s="21"/>
       <c r="C88" s="21"/>
@@ -4284,7 +4322,7 @@
       <c r="N88" s="8"/>
       <c r="O88" s="1"/>
     </row>
-    <row r="89" spans="1:15" ht="13.5" thickBot="1">
+    <row r="89" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A89" s="1"/>
       <c r="B89" s="21"/>
       <c r="C89" s="21"/>
@@ -4310,7 +4348,7 @@
       <c r="N89" s="8"/>
       <c r="O89" s="1"/>
     </row>
-    <row r="90" spans="1:15" ht="13.5" thickBot="1">
+    <row r="90" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A90" s="1"/>
       <c r="B90" s="21"/>
       <c r="C90" s="21"/>
@@ -4336,7 +4374,7 @@
       <c r="N90" s="8"/>
       <c r="O90" s="1"/>
     </row>
-    <row r="91" spans="1:15" ht="13.5" thickBot="1">
+    <row r="91" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A91" s="1"/>
       <c r="B91" s="21"/>
       <c r="C91" s="21"/>
@@ -4362,7 +4400,7 @@
       <c r="N91" s="8"/>
       <c r="O91" s="1"/>
     </row>
-    <row r="92" spans="1:15" ht="13.5" thickBot="1">
+    <row r="92" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A92" s="1"/>
       <c r="B92" s="21"/>
       <c r="C92" s="21"/>
@@ -4388,7 +4426,7 @@
       <c r="N92" s="8"/>
       <c r="O92" s="1"/>
     </row>
-    <row r="93" spans="1:15" ht="13.5" thickBot="1">
+    <row r="93" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A93" s="1"/>
       <c r="B93" s="21"/>
       <c r="C93" s="21"/>
@@ -4414,7 +4452,7 @@
       <c r="N93" s="8"/>
       <c r="O93" s="1"/>
     </row>
-    <row r="94" spans="1:15" ht="13.5" thickBot="1">
+    <row r="94" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A94" s="1"/>
       <c r="B94" s="21"/>
       <c r="C94" s="21"/>
@@ -4440,7 +4478,7 @@
       <c r="N94" s="8"/>
       <c r="O94" s="1"/>
     </row>
-    <row r="95" spans="1:15" ht="13.5" thickBot="1">
+    <row r="95" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A95" s="1"/>
       <c r="B95" s="21"/>
       <c r="C95" s="21"/>
@@ -4466,7 +4504,7 @@
       <c r="N95" s="8"/>
       <c r="O95" s="1"/>
     </row>
-    <row r="96" spans="1:15" ht="13.5" thickBot="1">
+    <row r="96" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A96" s="1"/>
       <c r="B96" s="21"/>
       <c r="C96" s="21"/>
@@ -4492,7 +4530,7 @@
       <c r="N96" s="8"/>
       <c r="O96" s="1"/>
     </row>
-    <row r="97" spans="1:15" ht="13.5" thickBot="1">
+    <row r="97" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A97" s="1"/>
       <c r="B97" s="21"/>
       <c r="C97" s="21"/>
@@ -4518,7 +4556,7 @@
       <c r="N97" s="8"/>
       <c r="O97" s="1"/>
     </row>
-    <row r="98" spans="1:15" ht="13.5" thickBot="1">
+    <row r="98" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A98" s="1"/>
       <c r="B98" s="21"/>
       <c r="C98" s="21"/>
@@ -4544,7 +4582,7 @@
       <c r="N98" s="8"/>
       <c r="O98" s="1"/>
     </row>
-    <row r="99" spans="1:15" ht="13.5" thickBot="1">
+    <row r="99" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A99" s="1"/>
       <c r="B99" s="21"/>
       <c r="C99" s="21"/>
@@ -4570,7 +4608,7 @@
       <c r="N99" s="8"/>
       <c r="O99" s="1"/>
     </row>
-    <row r="100" spans="1:15" ht="13.5" thickBot="1">
+    <row r="100" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A100" s="1"/>
       <c r="B100" s="21"/>
       <c r="C100" s="21"/>
@@ -4596,7 +4634,7 @@
       <c r="N100" s="8"/>
       <c r="O100" s="1"/>
     </row>
-    <row r="101" spans="1:15" ht="13.5" thickBot="1">
+    <row r="101" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A101" s="1"/>
       <c r="B101" s="21"/>
       <c r="C101" s="21"/>
@@ -4622,7 +4660,7 @@
       <c r="N101" s="8"/>
       <c r="O101" s="1"/>
     </row>
-    <row r="102" spans="1:15" ht="13.5" thickBot="1">
+    <row r="102" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A102" s="1"/>
       <c r="B102" s="21"/>
       <c r="C102" s="21"/>
@@ -4648,7 +4686,7 @@
       <c r="N102" s="8"/>
       <c r="O102" s="1"/>
     </row>
-    <row r="103" spans="1:15" ht="13.5" thickBot="1">
+    <row r="103" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A103" s="1"/>
       <c r="B103" s="21"/>
       <c r="C103" s="21"/>
@@ -4674,7 +4712,7 @@
       <c r="N103" s="8"/>
       <c r="O103" s="1"/>
     </row>
-    <row r="104" spans="1:15" ht="13.5" thickBot="1">
+    <row r="104" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A104" s="1"/>
       <c r="B104" s="21"/>
       <c r="C104" s="21"/>
@@ -4700,7 +4738,7 @@
       <c r="N104" s="8"/>
       <c r="O104" s="1"/>
     </row>
-    <row r="105" spans="1:15" ht="13.5" thickBot="1">
+    <row r="105" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A105" s="1"/>
       <c r="B105" s="21"/>
       <c r="C105" s="21"/>
@@ -4726,7 +4764,7 @@
       <c r="N105" s="8"/>
       <c r="O105" s="1"/>
     </row>
-    <row r="106" spans="1:15" ht="13.5" thickBot="1">
+    <row r="106" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A106" s="1"/>
       <c r="B106" s="21"/>
       <c r="C106" s="21"/>
@@ -4752,7 +4790,7 @@
       <c r="N106" s="8"/>
       <c r="O106" s="1"/>
     </row>
-    <row r="107" spans="1:15" ht="13.5" thickBot="1">
+    <row r="107" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A107" s="1"/>
       <c r="B107" s="21"/>
       <c r="C107" s="21"/>
@@ -4778,7 +4816,7 @@
       <c r="N107" s="8"/>
       <c r="O107" s="1"/>
     </row>
-    <row r="108" spans="1:15" ht="13.5" thickBot="1">
+    <row r="108" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A108" s="1"/>
       <c r="B108" s="21"/>
       <c r="C108" s="21"/>
@@ -4804,7 +4842,7 @@
       <c r="N108" s="8"/>
       <c r="O108" s="1"/>
     </row>
-    <row r="109" spans="1:15" ht="13.5" thickBot="1">
+    <row r="109" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A109" s="1"/>
       <c r="B109" s="21"/>
       <c r="C109" s="21"/>
@@ -4830,7 +4868,7 @@
       <c r="N109" s="8"/>
       <c r="O109" s="1"/>
     </row>
-    <row r="110" spans="1:15" ht="13.5" thickBot="1">
+    <row r="110" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A110" s="1"/>
       <c r="B110" s="21"/>
       <c r="C110" s="21"/>
@@ -4856,7 +4894,7 @@
       <c r="N110" s="8"/>
       <c r="O110" s="1"/>
     </row>
-    <row r="111" spans="1:15" ht="13.5" thickBot="1">
+    <row r="111" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A111" s="1"/>
       <c r="B111" s="21"/>
       <c r="C111" s="21"/>
@@ -4882,7 +4920,7 @@
       <c r="N111" s="8"/>
       <c r="O111" s="1"/>
     </row>
-    <row r="112" spans="1:15" ht="13.5" thickBot="1">
+    <row r="112" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A112" s="1"/>
       <c r="B112" s="21"/>
       <c r="C112" s="21"/>
@@ -4908,7 +4946,7 @@
       <c r="N112" s="8"/>
       <c r="O112" s="1"/>
     </row>
-    <row r="113" spans="1:15" ht="13.5" thickBot="1">
+    <row r="113" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A113" s="1"/>
       <c r="B113" s="21"/>
       <c r="C113" s="21"/>
@@ -4934,7 +4972,7 @@
       <c r="N113" s="8"/>
       <c r="O113" s="1"/>
     </row>
-    <row r="114" spans="1:15" ht="13.5" thickBot="1">
+    <row r="114" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A114" s="1"/>
       <c r="B114" s="21"/>
       <c r="C114" s="21"/>
@@ -4960,7 +4998,7 @@
       <c r="N114" s="8"/>
       <c r="O114" s="1"/>
     </row>
-    <row r="115" spans="1:15" ht="13.5" thickBot="1">
+    <row r="115" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A115" s="1"/>
       <c r="B115" s="21"/>
       <c r="C115" s="21"/>
@@ -4986,7 +5024,7 @@
       <c r="N115" s="8"/>
       <c r="O115" s="1"/>
     </row>
-    <row r="116" spans="1:15" ht="13.5" thickBot="1">
+    <row r="116" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A116" s="1"/>
       <c r="B116" s="21"/>
       <c r="C116" s="21"/>
@@ -5012,7 +5050,7 @@
       <c r="N116" s="8"/>
       <c r="O116" s="1"/>
     </row>
-    <row r="117" spans="1:15" ht="13.5" thickBot="1">
+    <row r="117" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A117" s="1"/>
       <c r="B117" s="21"/>
       <c r="C117" s="21"/>
@@ -5038,7 +5076,7 @@
       <c r="N117" s="8"/>
       <c r="O117" s="1"/>
     </row>
-    <row r="118" spans="1:15" ht="13.5" thickBot="1">
+    <row r="118" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A118" s="1"/>
       <c r="B118" s="21"/>
       <c r="C118" s="21"/>
@@ -5064,7 +5102,7 @@
       <c r="N118" s="8"/>
       <c r="O118" s="1"/>
     </row>
-    <row r="119" spans="1:15" ht="13.5" thickBot="1">
+    <row r="119" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A119" s="1"/>
       <c r="B119" s="21"/>
       <c r="C119" s="21"/>
@@ -5090,7 +5128,7 @@
       <c r="N119" s="8"/>
       <c r="O119" s="1"/>
     </row>
-    <row r="120" spans="1:15" ht="13.5" thickBot="1">
+    <row r="120" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A120" s="1"/>
       <c r="B120" s="21"/>
       <c r="C120" s="21"/>
@@ -5116,7 +5154,7 @@
       <c r="N120" s="8"/>
       <c r="O120" s="1"/>
     </row>
-    <row r="121" spans="1:15" ht="13.5" thickBot="1">
+    <row r="121" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A121" s="1"/>
       <c r="B121" s="21"/>
       <c r="C121" s="21"/>
@@ -5142,7 +5180,7 @@
       <c r="N121" s="8"/>
       <c r="O121" s="1"/>
     </row>
-    <row r="122" spans="1:15" ht="13.5" thickBot="1">
+    <row r="122" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A122" s="1"/>
       <c r="B122" s="21"/>
       <c r="C122" s="21"/>
@@ -5168,7 +5206,7 @@
       <c r="N122" s="8"/>
       <c r="O122" s="1"/>
     </row>
-    <row r="123" spans="1:15" ht="13.5" thickBot="1">
+    <row r="123" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A123" s="1"/>
       <c r="B123" s="21"/>
       <c r="C123" s="21"/>
@@ -5194,7 +5232,7 @@
       <c r="N123" s="8"/>
       <c r="O123" s="1"/>
     </row>
-    <row r="124" spans="1:15" ht="13.5" thickBot="1">
+    <row r="124" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A124" s="1"/>
       <c r="B124" s="21"/>
       <c r="C124" s="21"/>
@@ -5220,7 +5258,7 @@
       <c r="N124" s="8"/>
       <c r="O124" s="1"/>
     </row>
-    <row r="125" spans="1:15" ht="13.5" thickBot="1">
+    <row r="125" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A125" s="1"/>
       <c r="B125" s="21"/>
       <c r="C125" s="21"/>
@@ -5246,7 +5284,7 @@
       <c r="N125" s="8"/>
       <c r="O125" s="1"/>
     </row>
-    <row r="126" spans="1:15" ht="13.5" thickBot="1">
+    <row r="126" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A126" s="1"/>
       <c r="B126" s="21"/>
       <c r="C126" s="21"/>
@@ -5272,7 +5310,7 @@
       <c r="N126" s="8"/>
       <c r="O126" s="1"/>
     </row>
-    <row r="127" spans="1:15" ht="13.5" thickBot="1">
+    <row r="127" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A127" s="1"/>
       <c r="B127" s="21"/>
       <c r="C127" s="21"/>
@@ -5298,7 +5336,7 @@
       <c r="N127" s="8"/>
       <c r="O127" s="1"/>
     </row>
-    <row r="128" spans="1:15" ht="13.5" thickBot="1">
+    <row r="128" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A128" s="1"/>
       <c r="B128" s="21"/>
       <c r="C128" s="21"/>
@@ -5324,7 +5362,7 @@
       <c r="N128" s="8"/>
       <c r="O128" s="1"/>
     </row>
-    <row r="129" spans="1:15" ht="13.5" thickBot="1">
+    <row r="129" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A129" s="1"/>
       <c r="B129" s="21"/>
       <c r="C129" s="21"/>
@@ -5350,7 +5388,7 @@
       <c r="N129" s="8"/>
       <c r="O129" s="1"/>
     </row>
-    <row r="130" spans="1:15" ht="13.5" thickBot="1">
+    <row r="130" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A130" s="1"/>
       <c r="B130" s="21"/>
       <c r="C130" s="21"/>
@@ -5376,7 +5414,7 @@
       <c r="N130" s="8"/>
       <c r="O130" s="1"/>
     </row>
-    <row r="131" spans="1:15" ht="13.5" thickBot="1">
+    <row r="131" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A131" s="1"/>
       <c r="B131" s="21"/>
       <c r="C131" s="21"/>
@@ -5402,7 +5440,7 @@
       <c r="N131" s="8"/>
       <c r="O131" s="1"/>
     </row>
-    <row r="132" spans="1:15" ht="13.5" thickBot="1">
+    <row r="132" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A132" s="1"/>
       <c r="B132" s="21"/>
       <c r="C132" s="21"/>
@@ -5428,7 +5466,7 @@
       <c r="N132" s="8"/>
       <c r="O132" s="1"/>
     </row>
-    <row r="133" spans="1:15" ht="13.5" thickBot="1">
+    <row r="133" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A133" s="1"/>
       <c r="B133" s="21"/>
       <c r="C133" s="21"/>
@@ -5454,7 +5492,7 @@
       <c r="N133" s="8"/>
       <c r="O133" s="1"/>
     </row>
-    <row r="134" spans="1:15" ht="13.5" thickBot="1">
+    <row r="134" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A134" s="1"/>
       <c r="B134" s="21"/>
       <c r="C134" s="21"/>
@@ -5480,7 +5518,7 @@
       <c r="N134" s="8"/>
       <c r="O134" s="1"/>
     </row>
-    <row r="135" spans="1:15" ht="13.5" thickBot="1">
+    <row r="135" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A135" s="1"/>
       <c r="B135" s="21"/>
       <c r="C135" s="21"/>
@@ -5506,7 +5544,7 @@
       <c r="N135" s="8"/>
       <c r="O135" s="1"/>
     </row>
-    <row r="136" spans="1:15" ht="13.5" thickBot="1">
+    <row r="136" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A136" s="1"/>
       <c r="B136" s="21"/>
       <c r="C136" s="21"/>
@@ -5532,7 +5570,7 @@
       <c r="N136" s="8"/>
       <c r="O136" s="1"/>
     </row>
-    <row r="137" spans="1:15" ht="13.5" thickBot="1">
+    <row r="137" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A137" s="1"/>
       <c r="B137" s="21"/>
       <c r="C137" s="21"/>
@@ -5558,7 +5596,7 @@
       <c r="N137" s="8"/>
       <c r="O137" s="1"/>
     </row>
-    <row r="138" spans="1:15" ht="13.5" thickBot="1">
+    <row r="138" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A138" s="1"/>
       <c r="B138" s="21"/>
       <c r="C138" s="21"/>
@@ -5584,7 +5622,7 @@
       <c r="N138" s="8"/>
       <c r="O138" s="1"/>
     </row>
-    <row r="139" spans="1:15" ht="13.5" thickBot="1">
+    <row r="139" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A139" s="1"/>
       <c r="B139" s="21"/>
       <c r="C139" s="21"/>
@@ -5610,7 +5648,7 @@
       <c r="N139" s="8"/>
       <c r="O139" s="1"/>
     </row>
-    <row r="140" spans="1:15" ht="13.5" thickBot="1">
+    <row r="140" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A140" s="1"/>
       <c r="B140" s="21"/>
       <c r="C140" s="21"/>
@@ -5636,7 +5674,7 @@
       <c r="N140" s="8"/>
       <c r="O140" s="1"/>
     </row>
-    <row r="141" spans="1:15" ht="13.5" thickBot="1">
+    <row r="141" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A141" s="1"/>
       <c r="B141" s="21"/>
       <c r="C141" s="21"/>
@@ -5662,7 +5700,7 @@
       <c r="N141" s="8"/>
       <c r="O141" s="1"/>
     </row>
-    <row r="142" spans="1:15" ht="13.5" thickBot="1">
+    <row r="142" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A142" s="1"/>
       <c r="B142" s="21"/>
       <c r="C142" s="21"/>
@@ -5688,7 +5726,7 @@
       <c r="N142" s="8"/>
       <c r="O142" s="1"/>
     </row>
-    <row r="143" spans="1:15" ht="13.5" thickBot="1">
+    <row r="143" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A143" s="1"/>
       <c r="B143" s="21"/>
       <c r="C143" s="21"/>
@@ -5714,7 +5752,7 @@
       <c r="N143" s="8"/>
       <c r="O143" s="1"/>
     </row>
-    <row r="144" spans="1:15" ht="13.5" thickBot="1">
+    <row r="144" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A144" s="1"/>
       <c r="B144" s="21"/>
       <c r="C144" s="21"/>
@@ -5740,7 +5778,7 @@
       <c r="N144" s="8"/>
       <c r="O144" s="1"/>
     </row>
-    <row r="145" spans="1:15" ht="13.5" thickBot="1">
+    <row r="145" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A145" s="1"/>
       <c r="B145" s="21"/>
       <c r="C145" s="21"/>
@@ -5766,7 +5804,7 @@
       <c r="N145" s="8"/>
       <c r="O145" s="1"/>
     </row>
-    <row r="146" spans="1:15" ht="13.5" thickBot="1">
+    <row r="146" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A146" s="1"/>
       <c r="B146" s="21"/>
       <c r="C146" s="21"/>
@@ -5792,7 +5830,7 @@
       <c r="N146" s="8"/>
       <c r="O146" s="1"/>
     </row>
-    <row r="147" spans="1:15" ht="13.5" thickBot="1">
+    <row r="147" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A147" s="1"/>
       <c r="B147" s="21"/>
       <c r="C147" s="21"/>
@@ -5818,7 +5856,7 @@
       <c r="N147" s="8"/>
       <c r="O147" s="1"/>
     </row>
-    <row r="148" spans="1:15" ht="13.5" thickBot="1">
+    <row r="148" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A148" s="1"/>
       <c r="B148" s="21"/>
       <c r="C148" s="21"/>
@@ -5844,7 +5882,7 @@
       <c r="N148" s="8"/>
       <c r="O148" s="1"/>
     </row>
-    <row r="149" spans="1:15" ht="13.5" thickBot="1">
+    <row r="149" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A149" s="1"/>
       <c r="B149" s="21"/>
       <c r="C149" s="21"/>
@@ -5870,7 +5908,7 @@
       <c r="N149" s="8"/>
       <c r="O149" s="1"/>
     </row>
-    <row r="150" spans="1:15" ht="13.5" thickBot="1">
+    <row r="150" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A150" s="1"/>
       <c r="B150" s="21"/>
       <c r="C150" s="21"/>
@@ -5896,7 +5934,7 @@
       <c r="N150" s="8"/>
       <c r="O150" s="1"/>
     </row>
-    <row r="151" spans="1:15" ht="13.5" thickBot="1">
+    <row r="151" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A151" s="1"/>
       <c r="B151" s="21"/>
       <c r="C151" s="21"/>
@@ -5922,7 +5960,7 @@
       <c r="N151" s="8"/>
       <c r="O151" s="1"/>
     </row>
-    <row r="152" spans="1:15" ht="13.5" thickBot="1">
+    <row r="152" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A152" s="1"/>
       <c r="B152" s="21"/>
       <c r="C152" s="21"/>
@@ -5948,7 +5986,7 @@
       <c r="N152" s="8"/>
       <c r="O152" s="1"/>
     </row>
-    <row r="153" spans="1:15" ht="13.5" thickBot="1">
+    <row r="153" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A153" s="1"/>
       <c r="B153" s="21"/>
       <c r="C153" s="21"/>
@@ -5974,7 +6012,7 @@
       <c r="N153" s="8"/>
       <c r="O153" s="1"/>
     </row>
-    <row r="154" spans="1:15" ht="13.5" thickBot="1">
+    <row r="154" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A154" s="1"/>
       <c r="B154" s="21"/>
       <c r="C154" s="21"/>
@@ -6000,7 +6038,7 @@
       <c r="N154" s="8"/>
       <c r="O154" s="1"/>
     </row>
-    <row r="155" spans="1:15" ht="13.5" thickBot="1">
+    <row r="155" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A155" s="1"/>
       <c r="B155" s="21"/>
       <c r="C155" s="21"/>
@@ -6026,7 +6064,7 @@
       <c r="N155" s="8"/>
       <c r="O155" s="1"/>
     </row>
-    <row r="156" spans="1:15" ht="13.5" thickBot="1">
+    <row r="156" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A156" s="1"/>
       <c r="B156" s="21"/>
       <c r="C156" s="21"/>
@@ -6052,7 +6090,7 @@
       <c r="N156" s="8"/>
       <c r="O156" s="1"/>
     </row>
-    <row r="157" spans="1:15" ht="13.5" thickBot="1">
+    <row r="157" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A157" s="1"/>
       <c r="B157" s="21"/>
       <c r="C157" s="21"/>
@@ -6078,7 +6116,7 @@
       <c r="N157" s="8"/>
       <c r="O157" s="1"/>
     </row>
-    <row r="158" spans="1:15" ht="13.5" thickBot="1">
+    <row r="158" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A158" s="1"/>
       <c r="B158" s="21"/>
       <c r="C158" s="21"/>
@@ -6104,7 +6142,7 @@
       <c r="N158" s="8"/>
       <c r="O158" s="1"/>
     </row>
-    <row r="159" spans="1:15" ht="13.5" thickBot="1">
+    <row r="159" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A159" s="1"/>
       <c r="B159" s="21"/>
       <c r="C159" s="21"/>
@@ -6130,7 +6168,7 @@
       <c r="N159" s="8"/>
       <c r="O159" s="1"/>
     </row>
-    <row r="160" spans="1:15" ht="13.5" thickBot="1">
+    <row r="160" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A160" s="1"/>
       <c r="B160" s="21"/>
       <c r="C160" s="21"/>
@@ -6156,7 +6194,7 @@
       <c r="N160" s="8"/>
       <c r="O160" s="1"/>
     </row>
-    <row r="161" spans="1:15" ht="13.5" thickBot="1">
+    <row r="161" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A161" s="1"/>
       <c r="B161" s="21"/>
       <c r="C161" s="21"/>
@@ -6182,7 +6220,7 @@
       <c r="N161" s="8"/>
       <c r="O161" s="1"/>
     </row>
-    <row r="162" spans="1:15" ht="13.5" thickBot="1">
+    <row r="162" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A162" s="1"/>
       <c r="B162" s="21"/>
       <c r="C162" s="21"/>
@@ -6208,7 +6246,7 @@
       <c r="N162" s="8"/>
       <c r="O162" s="1"/>
     </row>
-    <row r="163" spans="1:15" ht="13.5" thickBot="1">
+    <row r="163" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A163" s="1"/>
       <c r="B163" s="21"/>
       <c r="C163" s="21"/>
@@ -6234,7 +6272,7 @@
       <c r="N163" s="8"/>
       <c r="O163" s="1"/>
     </row>
-    <row r="164" spans="1:15" ht="13.5" thickBot="1">
+    <row r="164" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A164" s="1"/>
       <c r="B164" s="21"/>
       <c r="C164" s="21"/>
@@ -6260,7 +6298,7 @@
       <c r="N164" s="8"/>
       <c r="O164" s="1"/>
     </row>
-    <row r="165" spans="1:15" ht="13.5" thickBot="1">
+    <row r="165" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A165" s="1"/>
       <c r="B165" s="21"/>
       <c r="C165" s="21"/>
@@ -6286,7 +6324,7 @@
       <c r="N165" s="8"/>
       <c r="O165" s="1"/>
     </row>
-    <row r="166" spans="1:15" ht="13.5" thickBot="1">
+    <row r="166" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A166" s="1"/>
       <c r="B166" s="21"/>
       <c r="C166" s="21"/>
@@ -6312,7 +6350,7 @@
       <c r="N166" s="8"/>
       <c r="O166" s="1"/>
     </row>
-    <row r="167" spans="1:15" ht="13.5" thickBot="1">
+    <row r="167" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A167" s="1"/>
       <c r="B167" s="21"/>
       <c r="C167" s="21"/>
@@ -6338,7 +6376,7 @@
       <c r="N167" s="8"/>
       <c r="O167" s="1"/>
     </row>
-    <row r="168" spans="1:15" ht="13.5" thickBot="1">
+    <row r="168" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A168" s="1"/>
       <c r="B168" s="21"/>
       <c r="C168" s="21"/>
@@ -6364,7 +6402,7 @@
       <c r="N168" s="8"/>
       <c r="O168" s="1"/>
     </row>
-    <row r="169" spans="1:15" ht="13.5" thickBot="1">
+    <row r="169" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A169" s="1"/>
       <c r="B169" s="21"/>
       <c r="C169" s="21"/>
@@ -6390,7 +6428,7 @@
       <c r="N169" s="8"/>
       <c r="O169" s="1"/>
     </row>
-    <row r="170" spans="1:15" ht="13.5" thickBot="1">
+    <row r="170" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A170" s="1"/>
       <c r="B170" s="21"/>
       <c r="C170" s="21"/>
@@ -6416,7 +6454,7 @@
       <c r="N170" s="8"/>
       <c r="O170" s="1"/>
     </row>
-    <row r="171" spans="1:15" ht="13.5" thickBot="1">
+    <row r="171" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A171" s="1"/>
       <c r="B171" s="21"/>
       <c r="C171" s="21"/>
@@ -6442,7 +6480,7 @@
       <c r="N171" s="8"/>
       <c r="O171" s="1"/>
     </row>
-    <row r="172" spans="1:15" ht="13.5" thickBot="1">
+    <row r="172" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A172" s="1"/>
       <c r="B172" s="21"/>
       <c r="C172" s="21"/>
@@ -6468,7 +6506,7 @@
       <c r="N172" s="8"/>
       <c r="O172" s="1"/>
     </row>
-    <row r="173" spans="1:15" ht="13.5" thickBot="1">
+    <row r="173" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A173" s="1"/>
       <c r="B173" s="21"/>
       <c r="C173" s="21"/>
@@ -6494,7 +6532,7 @@
       <c r="N173" s="8"/>
       <c r="O173" s="1"/>
     </row>
-    <row r="174" spans="1:15" ht="13.5" thickBot="1">
+    <row r="174" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A174" s="1"/>
       <c r="B174" s="21"/>
       <c r="C174" s="21"/>
@@ -6520,7 +6558,7 @@
       <c r="N174" s="8"/>
       <c r="O174" s="1"/>
     </row>
-    <row r="175" spans="1:15" ht="13.5" thickBot="1">
+    <row r="175" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A175" s="1"/>
       <c r="B175" s="21"/>
       <c r="C175" s="21"/>
@@ -6546,7 +6584,7 @@
       <c r="N175" s="8"/>
       <c r="O175" s="1"/>
     </row>
-    <row r="176" spans="1:15" ht="13.5" thickBot="1">
+    <row r="176" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A176" s="1"/>
       <c r="B176" s="21"/>
       <c r="C176" s="21"/>
@@ -6572,7 +6610,7 @@
       <c r="N176" s="8"/>
       <c r="O176" s="1"/>
     </row>
-    <row r="177" spans="1:15" ht="13.5" thickBot="1">
+    <row r="177" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A177" s="1"/>
       <c r="B177" s="21"/>
       <c r="C177" s="21"/>
@@ -6598,7 +6636,7 @@
       <c r="N177" s="8"/>
       <c r="O177" s="1"/>
     </row>
-    <row r="178" spans="1:15" ht="13.5" thickBot="1">
+    <row r="178" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A178" s="1"/>
       <c r="B178" s="21"/>
       <c r="C178" s="21"/>
@@ -6624,7 +6662,7 @@
       <c r="N178" s="8"/>
       <c r="O178" s="1"/>
     </row>
-    <row r="179" spans="1:15" ht="13.5" thickBot="1">
+    <row r="179" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A179" s="1"/>
       <c r="B179" s="21"/>
       <c r="C179" s="21"/>
@@ -6650,7 +6688,7 @@
       <c r="N179" s="8"/>
       <c r="O179" s="1"/>
     </row>
-    <row r="180" spans="1:15" ht="13.5" thickBot="1">
+    <row r="180" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A180" s="1"/>
       <c r="B180" s="21"/>
       <c r="C180" s="21"/>
@@ -6676,7 +6714,7 @@
       <c r="N180" s="8"/>
       <c r="O180" s="1"/>
     </row>
-    <row r="181" spans="1:15" ht="13.5" thickBot="1">
+    <row r="181" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A181" s="1"/>
       <c r="B181" s="21"/>
       <c r="C181" s="21"/>
@@ -6702,7 +6740,7 @@
       <c r="N181" s="8"/>
       <c r="O181" s="1"/>
     </row>
-    <row r="182" spans="1:15" ht="13.5" thickBot="1">
+    <row r="182" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A182" s="1"/>
       <c r="B182" s="21"/>
       <c r="C182" s="21"/>
@@ -6728,7 +6766,7 @@
       <c r="N182" s="8"/>
       <c r="O182" s="1"/>
     </row>
-    <row r="183" spans="1:15" ht="13.5" thickBot="1">
+    <row r="183" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A183" s="1"/>
       <c r="B183" s="21"/>
       <c r="C183" s="21"/>
@@ -6754,7 +6792,7 @@
       <c r="N183" s="8"/>
       <c r="O183" s="1"/>
     </row>
-    <row r="184" spans="1:15" ht="13.5" thickBot="1">
+    <row r="184" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A184" s="1"/>
       <c r="B184" s="21"/>
       <c r="C184" s="21"/>
@@ -6780,7 +6818,7 @@
       <c r="N184" s="8"/>
       <c r="O184" s="1"/>
     </row>
-    <row r="185" spans="1:15" ht="13.5" thickBot="1">
+    <row r="185" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A185" s="1"/>
       <c r="B185" s="21"/>
       <c r="C185" s="21"/>
@@ -6806,7 +6844,7 @@
       <c r="N185" s="8"/>
       <c r="O185" s="1"/>
     </row>
-    <row r="186" spans="1:15" ht="13.5" thickBot="1">
+    <row r="186" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A186" s="1"/>
       <c r="B186" s="21"/>
       <c r="C186" s="21"/>
@@ -6832,7 +6870,7 @@
       <c r="N186" s="8"/>
       <c r="O186" s="1"/>
     </row>
-    <row r="187" spans="1:15" ht="13.5" thickBot="1">
+    <row r="187" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A187" s="1"/>
       <c r="B187" s="21"/>
       <c r="C187" s="21"/>
@@ -6858,7 +6896,7 @@
       <c r="N187" s="8"/>
       <c r="O187" s="1"/>
     </row>
-    <row r="188" spans="1:15" ht="13.5" thickBot="1">
+    <row r="188" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A188" s="1"/>
       <c r="B188" s="21"/>
       <c r="C188" s="21"/>
@@ -6884,7 +6922,7 @@
       <c r="N188" s="8"/>
       <c r="O188" s="1"/>
     </row>
-    <row r="189" spans="1:15" ht="13.5" thickBot="1">
+    <row r="189" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A189" s="1"/>
       <c r="B189" s="21"/>
       <c r="C189" s="21"/>
@@ -6910,7 +6948,7 @@
       <c r="N189" s="8"/>
       <c r="O189" s="1"/>
     </row>
-    <row r="190" spans="1:15" ht="13.5" thickBot="1">
+    <row r="190" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A190" s="1"/>
       <c r="B190" s="21"/>
       <c r="C190" s="21"/>
@@ -6936,7 +6974,7 @@
       <c r="N190" s="8"/>
       <c r="O190" s="1"/>
     </row>
-    <row r="191" spans="1:15" ht="13.5" thickBot="1">
+    <row r="191" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A191" s="1"/>
       <c r="B191" s="21"/>
       <c r="C191" s="21"/>
@@ -6962,7 +7000,7 @@
       <c r="N191" s="8"/>
       <c r="O191" s="1"/>
     </row>
-    <row r="192" spans="1:15" ht="13.5" thickBot="1">
+    <row r="192" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A192" s="1"/>
       <c r="B192" s="21"/>
       <c r="C192" s="21"/>
@@ -6988,7 +7026,7 @@
       <c r="N192" s="8"/>
       <c r="O192" s="1"/>
     </row>
-    <row r="193" spans="1:15" ht="13.5" thickBot="1">
+    <row r="193" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A193" s="1"/>
       <c r="B193" s="21"/>
       <c r="C193" s="21"/>
@@ -7014,7 +7052,7 @@
       <c r="N193" s="8"/>
       <c r="O193" s="1"/>
     </row>
-    <row r="194" spans="1:15" ht="13.5" thickBot="1">
+    <row r="194" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A194" s="1"/>
       <c r="B194" s="21"/>
       <c r="C194" s="21"/>
@@ -7040,7 +7078,7 @@
       <c r="N194" s="8"/>
       <c r="O194" s="1"/>
     </row>
-    <row r="195" spans="1:15" ht="13.5" thickBot="1">
+    <row r="195" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A195" s="1"/>
       <c r="B195" s="21"/>
       <c r="C195" s="21"/>
@@ -7066,7 +7104,7 @@
       <c r="N195" s="8"/>
       <c r="O195" s="1"/>
     </row>
-    <row r="196" spans="1:15" ht="13.5" thickBot="1">
+    <row r="196" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A196" s="1"/>
       <c r="B196" s="21"/>
       <c r="C196" s="21"/>
@@ -7092,7 +7130,7 @@
       <c r="N196" s="8"/>
       <c r="O196" s="1"/>
     </row>
-    <row r="197" spans="1:15" ht="13.5" thickBot="1">
+    <row r="197" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A197" s="1"/>
       <c r="B197" s="21"/>
       <c r="C197" s="21"/>
@@ -7118,7 +7156,7 @@
       <c r="N197" s="8"/>
       <c r="O197" s="1"/>
     </row>
-    <row r="198" spans="1:15" ht="13.5" thickBot="1">
+    <row r="198" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A198" s="1"/>
       <c r="B198" s="21"/>
       <c r="C198" s="21"/>
@@ -7144,7 +7182,7 @@
       <c r="N198" s="8"/>
       <c r="O198" s="1"/>
     </row>
-    <row r="199" spans="1:15" ht="13.5" thickBot="1">
+    <row r="199" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A199" s="1"/>
       <c r="B199" s="21"/>
       <c r="C199" s="21"/>
@@ -7170,7 +7208,7 @@
       <c r="N199" s="8"/>
       <c r="O199" s="1"/>
     </row>
-    <row r="200" spans="1:15" ht="13.5" thickBot="1">
+    <row r="200" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A200" s="1"/>
       <c r="B200" s="21"/>
       <c r="C200" s="21"/>
@@ -7196,7 +7234,7 @@
       <c r="N200" s="8"/>
       <c r="O200" s="1"/>
     </row>
-    <row r="201" spans="1:15" ht="13.5" thickBot="1">
+    <row r="201" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A201" s="1"/>
       <c r="B201" s="21"/>
       <c r="C201" s="21"/>
@@ -7222,7 +7260,7 @@
       <c r="N201" s="8"/>
       <c r="O201" s="1"/>
     </row>
-    <row r="202" spans="1:15" ht="13.5" thickBot="1">
+    <row r="202" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A202" s="1"/>
       <c r="B202" s="21"/>
       <c r="C202" s="21"/>
@@ -7248,7 +7286,7 @@
       <c r="N202" s="8"/>
       <c r="O202" s="1"/>
     </row>
-    <row r="203" spans="1:15" ht="13.5" thickBot="1">
+    <row r="203" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A203" s="1"/>
       <c r="B203" s="21"/>
       <c r="C203" s="21"/>
@@ -7274,7 +7312,7 @@
       <c r="N203" s="8"/>
       <c r="O203" s="1"/>
     </row>
-    <row r="204" spans="1:15" ht="13.5" thickBot="1">
+    <row r="204" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A204" s="1"/>
       <c r="B204" s="21"/>
       <c r="C204" s="21"/>
@@ -7300,7 +7338,7 @@
       <c r="N204" s="8"/>
       <c r="O204" s="1"/>
     </row>
-    <row r="205" spans="1:15" ht="13.5" thickBot="1">
+    <row r="205" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A205" s="1"/>
       <c r="B205" s="21"/>
       <c r="C205" s="21"/>
@@ -7326,7 +7364,7 @@
       <c r="N205" s="8"/>
       <c r="O205" s="1"/>
     </row>
-    <row r="206" spans="1:15" ht="13.5" thickBot="1">
+    <row r="206" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A206" s="1"/>
       <c r="B206" s="21"/>
       <c r="C206" s="21"/>
@@ -7352,7 +7390,7 @@
       <c r="N206" s="8"/>
       <c r="O206" s="1"/>
     </row>
-    <row r="207" spans="1:15" ht="13.5" thickBot="1">
+    <row r="207" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A207" s="1"/>
       <c r="B207" s="21"/>
       <c r="C207" s="21"/>
@@ -7378,7 +7416,7 @@
       <c r="N207" s="8"/>
       <c r="O207" s="1"/>
     </row>
-    <row r="208" spans="1:15" ht="13.5" thickBot="1">
+    <row r="208" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A208" s="1"/>
       <c r="B208" s="21"/>
       <c r="C208" s="21"/>
@@ -7404,7 +7442,7 @@
       <c r="N208" s="8"/>
       <c r="O208" s="1"/>
     </row>
-    <row r="209" spans="1:15" ht="13.5" thickBot="1">
+    <row r="209" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A209" s="1"/>
       <c r="B209" s="21"/>
       <c r="C209" s="21"/>
@@ -7430,7 +7468,7 @@
       <c r="N209" s="8"/>
       <c r="O209" s="1"/>
     </row>
-    <row r="210" spans="1:15" ht="13.5" thickBot="1">
+    <row r="210" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A210" s="1"/>
       <c r="B210" s="21"/>
       <c r="C210" s="21"/>
@@ -7456,7 +7494,7 @@
       <c r="N210" s="8"/>
       <c r="O210" s="1"/>
     </row>
-    <row r="211" spans="1:15" ht="13.5" thickBot="1">
+    <row r="211" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A211" s="1"/>
       <c r="B211" s="21"/>
       <c r="C211" s="21"/>
@@ -7482,7 +7520,7 @@
       <c r="N211" s="8"/>
       <c r="O211" s="1"/>
     </row>
-    <row r="212" spans="1:15" ht="13.5" thickBot="1">
+    <row r="212" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A212" s="1"/>
       <c r="B212" s="21"/>
       <c r="C212" s="21"/>
@@ -7508,7 +7546,7 @@
       <c r="N212" s="8"/>
       <c r="O212" s="1"/>
     </row>
-    <row r="213" spans="1:15" ht="13.5" thickBot="1">
+    <row r="213" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A213" s="1"/>
       <c r="B213" s="21"/>
       <c r="C213" s="21"/>
@@ -7534,7 +7572,7 @@
       <c r="N213" s="8"/>
       <c r="O213" s="1"/>
     </row>
-    <row r="214" spans="1:15" ht="13.5" thickBot="1">
+    <row r="214" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A214" s="1"/>
       <c r="B214" s="21"/>
       <c r="C214" s="21"/>
@@ -7560,7 +7598,7 @@
       <c r="N214" s="8"/>
       <c r="O214" s="1"/>
     </row>
-    <row r="215" spans="1:15" ht="13.5" thickBot="1">
+    <row r="215" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A215" s="1"/>
       <c r="B215" s="21"/>
       <c r="C215" s="21"/>
@@ -7586,7 +7624,7 @@
       <c r="N215" s="8"/>
       <c r="O215" s="1"/>
     </row>
-    <row r="216" spans="1:15" ht="13.5" thickBot="1">
+    <row r="216" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A216" s="1"/>
       <c r="B216" s="21"/>
       <c r="C216" s="21"/>
@@ -7612,7 +7650,7 @@
       <c r="N216" s="8"/>
       <c r="O216" s="1"/>
     </row>
-    <row r="217" spans="1:15" ht="13.5" thickBot="1">
+    <row r="217" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A217" s="1"/>
       <c r="B217" s="21"/>
       <c r="C217" s="21"/>
@@ -7638,7 +7676,7 @@
       <c r="N217" s="8"/>
       <c r="O217" s="1"/>
     </row>
-    <row r="218" spans="1:15" ht="13.5" thickBot="1">
+    <row r="218" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A218" s="1"/>
       <c r="B218" s="21"/>
       <c r="C218" s="21"/>
@@ -7664,7 +7702,7 @@
       <c r="N218" s="8"/>
       <c r="O218" s="1"/>
     </row>
-    <row r="219" spans="1:15" ht="13.5" thickBot="1">
+    <row r="219" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A219" s="1"/>
       <c r="B219" s="21"/>
       <c r="C219" s="21"/>
@@ -7690,7 +7728,7 @@
       <c r="N219" s="8"/>
       <c r="O219" s="1"/>
     </row>
-    <row r="220" spans="1:15" ht="13.5" thickBot="1">
+    <row r="220" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A220" s="1"/>
       <c r="B220" s="21"/>
       <c r="C220" s="21"/>
@@ -7716,7 +7754,7 @@
       <c r="N220" s="8"/>
       <c r="O220" s="1"/>
     </row>
-    <row r="221" spans="1:15" ht="13.5" thickBot="1">
+    <row r="221" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A221" s="1"/>
       <c r="B221" s="21"/>
       <c r="C221" s="21"/>
@@ -7742,7 +7780,7 @@
       <c r="N221" s="8"/>
       <c r="O221" s="1"/>
     </row>
-    <row r="222" spans="1:15" ht="13.5" thickBot="1">
+    <row r="222" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A222" s="1"/>
       <c r="B222" s="21"/>
       <c r="C222" s="21"/>
@@ -7768,7 +7806,7 @@
       <c r="N222" s="8"/>
       <c r="O222" s="1"/>
     </row>
-    <row r="223" spans="1:15" ht="13.5" thickBot="1">
+    <row r="223" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A223" s="1"/>
       <c r="B223" s="21"/>
       <c r="C223" s="21"/>
@@ -7794,7 +7832,7 @@
       <c r="N223" s="8"/>
       <c r="O223" s="1"/>
     </row>
-    <row r="224" spans="1:15" ht="13.5" thickBot="1">
+    <row r="224" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A224" s="1"/>
       <c r="B224" s="21"/>
       <c r="C224" s="21"/>
@@ -7820,7 +7858,7 @@
       <c r="N224" s="8"/>
       <c r="O224" s="1"/>
     </row>
-    <row r="225" spans="1:15" ht="13.5" thickBot="1">
+    <row r="225" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A225" s="1"/>
       <c r="B225" s="21"/>
       <c r="C225" s="21"/>
@@ -7846,7 +7884,7 @@
       <c r="N225" s="8"/>
       <c r="O225" s="1"/>
     </row>
-    <row r="226" spans="1:15" ht="13.5" thickBot="1">
+    <row r="226" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A226" s="1"/>
       <c r="B226" s="21"/>
       <c r="C226" s="21"/>
@@ -7872,7 +7910,7 @@
       <c r="N226" s="8"/>
       <c r="O226" s="1"/>
     </row>
-    <row r="227" spans="1:15" ht="13.5" thickBot="1">
+    <row r="227" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A227" s="1"/>
       <c r="B227" s="21"/>
       <c r="C227" s="21"/>
@@ -7898,7 +7936,7 @@
       <c r="N227" s="8"/>
       <c r="O227" s="1"/>
     </row>
-    <row r="228" spans="1:15" ht="13.5" thickBot="1">
+    <row r="228" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A228" s="1"/>
       <c r="B228" s="21"/>
       <c r="C228" s="21"/>
@@ -7924,7 +7962,7 @@
       <c r="N228" s="8"/>
       <c r="O228" s="1"/>
     </row>
-    <row r="229" spans="1:15" ht="13.5" thickBot="1">
+    <row r="229" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A229" s="1"/>
       <c r="B229" s="21"/>
       <c r="C229" s="21"/>
@@ -7950,7 +7988,7 @@
       <c r="N229" s="8"/>
       <c r="O229" s="1"/>
     </row>
-    <row r="230" spans="1:15" ht="13.5" thickBot="1">
+    <row r="230" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A230" s="1"/>
       <c r="B230" s="21"/>
       <c r="C230" s="21"/>
@@ -7976,7 +8014,7 @@
       <c r="N230" s="8"/>
       <c r="O230" s="1"/>
     </row>
-    <row r="231" spans="1:15" ht="13.5" thickBot="1">
+    <row r="231" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A231" s="1"/>
       <c r="B231" s="21"/>
       <c r="C231" s="21"/>
@@ -8002,7 +8040,7 @@
       <c r="N231" s="8"/>
       <c r="O231" s="1"/>
     </row>
-    <row r="232" spans="1:15" ht="13.5" thickBot="1">
+    <row r="232" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A232" s="1"/>
       <c r="B232" s="21"/>
       <c r="C232" s="21"/>
@@ -8028,7 +8066,7 @@
       <c r="N232" s="8"/>
       <c r="O232" s="1"/>
     </row>
-    <row r="233" spans="1:15" ht="13.5" thickBot="1">
+    <row r="233" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A233" s="1"/>
       <c r="B233" s="21"/>
       <c r="C233" s="21"/>
@@ -8054,7 +8092,7 @@
       <c r="N233" s="8"/>
       <c r="O233" s="1"/>
     </row>
-    <row r="234" spans="1:15" ht="13.5" thickBot="1">
+    <row r="234" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A234" s="1"/>
       <c r="B234" s="21"/>
       <c r="C234" s="21"/>
@@ -8080,7 +8118,7 @@
       <c r="N234" s="8"/>
       <c r="O234" s="1"/>
     </row>
-    <row r="235" spans="1:15" ht="13.5" thickBot="1">
+    <row r="235" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A235" s="1"/>
       <c r="B235" s="21"/>
       <c r="C235" s="21"/>
@@ -8106,7 +8144,7 @@
       <c r="N235" s="8"/>
       <c r="O235" s="1"/>
     </row>
-    <row r="236" spans="1:15" ht="13.5" thickBot="1">
+    <row r="236" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A236" s="1"/>
       <c r="B236" s="21"/>
       <c r="C236" s="21"/>
@@ -8132,7 +8170,7 @@
       <c r="N236" s="8"/>
       <c r="O236" s="1"/>
     </row>
-    <row r="237" spans="1:15" ht="13.5" thickBot="1">
+    <row r="237" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A237" s="1"/>
       <c r="B237" s="21"/>
       <c r="C237" s="21"/>
@@ -8158,7 +8196,7 @@
       <c r="N237" s="8"/>
       <c r="O237" s="1"/>
     </row>
-    <row r="238" spans="1:15" ht="13.5" thickBot="1">
+    <row r="238" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A238" s="1"/>
       <c r="B238" s="21"/>
       <c r="C238" s="21"/>
@@ -8184,7 +8222,7 @@
       <c r="N238" s="8"/>
       <c r="O238" s="1"/>
     </row>
-    <row r="239" spans="1:15" ht="13.5" thickBot="1">
+    <row r="239" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A239" s="1"/>
       <c r="B239" s="21"/>
       <c r="C239" s="21"/>
@@ -8210,7 +8248,7 @@
       <c r="N239" s="8"/>
       <c r="O239" s="1"/>
     </row>
-    <row r="240" spans="1:15" ht="13.5" thickBot="1">
+    <row r="240" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A240" s="1"/>
       <c r="B240" s="21"/>
       <c r="C240" s="21"/>
@@ -8236,7 +8274,7 @@
       <c r="N240" s="8"/>
       <c r="O240" s="1"/>
     </row>
-    <row r="241" spans="1:15" ht="13.5" thickBot="1">
+    <row r="241" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A241" s="1"/>
       <c r="B241" s="21"/>
       <c r="C241" s="21"/>
@@ -8262,7 +8300,7 @@
       <c r="N241" s="8"/>
       <c r="O241" s="1"/>
     </row>
-    <row r="242" spans="1:15" ht="13.5" thickBot="1">
+    <row r="242" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A242" s="1"/>
       <c r="B242" s="21"/>
       <c r="C242" s="21"/>
@@ -8288,7 +8326,7 @@
       <c r="N242" s="8"/>
       <c r="O242" s="1"/>
     </row>
-    <row r="243" spans="1:15" ht="13.5" thickBot="1">
+    <row r="243" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A243" s="1"/>
       <c r="B243" s="21"/>
       <c r="C243" s="21"/>
@@ -8314,7 +8352,7 @@
       <c r="N243" s="8"/>
       <c r="O243" s="1"/>
     </row>
-    <row r="244" spans="1:15" ht="13.5" thickBot="1">
+    <row r="244" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A244" s="1"/>
       <c r="B244" s="21"/>
       <c r="C244" s="21"/>
@@ -8340,7 +8378,7 @@
       <c r="N244" s="8"/>
       <c r="O244" s="1"/>
     </row>
-    <row r="245" spans="1:15" ht="13.5" thickBot="1">
+    <row r="245" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A245" s="1"/>
       <c r="B245" s="21"/>
       <c r="C245" s="21"/>
@@ -8366,7 +8404,7 @@
       <c r="N245" s="8"/>
       <c r="O245" s="1"/>
     </row>
-    <row r="246" spans="1:15" ht="13.5" thickBot="1">
+    <row r="246" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A246" s="1"/>
       <c r="B246" s="21"/>
       <c r="C246" s="21"/>
@@ -8392,7 +8430,7 @@
       <c r="N246" s="8"/>
       <c r="O246" s="1"/>
     </row>
-    <row r="247" spans="1:15" ht="13.5" thickBot="1">
+    <row r="247" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A247" s="1"/>
       <c r="B247" s="21"/>
       <c r="C247" s="21"/>
@@ -8418,7 +8456,7 @@
       <c r="N247" s="8"/>
       <c r="O247" s="1"/>
     </row>
-    <row r="248" spans="1:15" ht="13.5" thickBot="1">
+    <row r="248" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A248" s="1"/>
       <c r="B248" s="21"/>
       <c r="C248" s="21"/>
@@ -8444,7 +8482,7 @@
       <c r="N248" s="8"/>
       <c r="O248" s="1"/>
     </row>
-    <row r="249" spans="1:15" ht="13.5" thickBot="1">
+    <row r="249" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A249" s="1"/>
       <c r="B249" s="21"/>
       <c r="C249" s="21"/>
@@ -8470,7 +8508,7 @@
       <c r="N249" s="8"/>
       <c r="O249" s="1"/>
     </row>
-    <row r="250" spans="1:15" ht="13.5" thickBot="1">
+    <row r="250" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A250" s="1"/>
       <c r="B250" s="21"/>
       <c r="C250" s="21"/>
@@ -8496,7 +8534,7 @@
       <c r="N250" s="8"/>
       <c r="O250" s="1"/>
     </row>
-    <row r="251" spans="1:15" ht="13.5" thickBot="1">
+    <row r="251" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A251" s="1"/>
       <c r="B251" s="21"/>
       <c r="C251" s="21"/>
@@ -8522,7 +8560,7 @@
       <c r="N251" s="8"/>
       <c r="O251" s="1"/>
     </row>
-    <row r="252" spans="1:15" ht="13.5" thickBot="1">
+    <row r="252" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A252" s="1"/>
       <c r="B252" s="21"/>
       <c r="C252" s="21"/>
@@ -8548,7 +8586,7 @@
       <c r="N252" s="8"/>
       <c r="O252" s="1"/>
     </row>
-    <row r="253" spans="1:15" ht="13.5" thickBot="1">
+    <row r="253" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A253" s="1"/>
       <c r="B253" s="21"/>
       <c r="C253" s="21"/>
@@ -8574,7 +8612,7 @@
       <c r="N253" s="8"/>
       <c r="O253" s="1"/>
     </row>
-    <row r="254" spans="1:15" ht="13.5" thickBot="1">
+    <row r="254" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A254" s="1"/>
       <c r="B254" s="21"/>
       <c r="C254" s="21"/>
@@ -8600,7 +8638,7 @@
       <c r="N254" s="8"/>
       <c r="O254" s="1"/>
     </row>
-    <row r="255" spans="1:15" ht="13.5" thickBot="1">
+    <row r="255" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A255" s="1"/>
       <c r="B255" s="21"/>
       <c r="C255" s="21"/>
@@ -8626,7 +8664,7 @@
       <c r="N255" s="8"/>
       <c r="O255" s="1"/>
     </row>
-    <row r="256" spans="1:15" ht="13.5" thickBot="1">
+    <row r="256" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A256" s="1"/>
       <c r="B256" s="21"/>
       <c r="C256" s="21"/>
@@ -8652,7 +8690,7 @@
       <c r="N256" s="8"/>
       <c r="O256" s="1"/>
     </row>
-    <row r="257" spans="1:15" ht="13.5" thickBot="1">
+    <row r="257" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A257" s="1"/>
       <c r="B257" s="21"/>
       <c r="C257" s="21"/>
@@ -8678,7 +8716,7 @@
       <c r="N257" s="8"/>
       <c r="O257" s="1"/>
     </row>
-    <row r="258" spans="1:15" ht="13.5" thickBot="1">
+    <row r="258" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A258" s="1"/>
       <c r="B258" s="21"/>
       <c r="C258" s="21"/>
@@ -8704,7 +8742,7 @@
       <c r="N258" s="8"/>
       <c r="O258" s="1"/>
     </row>
-    <row r="259" spans="1:15" ht="13.5" thickBot="1">
+    <row r="259" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A259" s="1"/>
       <c r="B259" s="21"/>
       <c r="C259" s="21"/>
@@ -8730,7 +8768,7 @@
       <c r="N259" s="8"/>
       <c r="O259" s="1"/>
     </row>
-    <row r="260" spans="1:15" ht="13.5" thickBot="1">
+    <row r="260" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A260" s="1"/>
       <c r="B260" s="21"/>
       <c r="C260" s="21"/>
@@ -8756,7 +8794,7 @@
       <c r="N260" s="8"/>
       <c r="O260" s="1"/>
     </row>
-    <row r="261" spans="1:15" ht="13.5" thickBot="1">
+    <row r="261" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A261" s="1"/>
       <c r="B261" s="21"/>
       <c r="C261" s="21"/>
@@ -8782,7 +8820,7 @@
       <c r="N261" s="8"/>
       <c r="O261" s="1"/>
     </row>
-    <row r="262" spans="1:15" ht="13.5" thickBot="1">
+    <row r="262" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A262" s="1"/>
       <c r="B262" s="21"/>
       <c r="C262" s="21"/>
@@ -8808,7 +8846,7 @@
       <c r="N262" s="8"/>
       <c r="O262" s="1"/>
     </row>
-    <row r="263" spans="1:15" ht="13.5" thickBot="1">
+    <row r="263" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A263" s="1"/>
       <c r="B263" s="21"/>
       <c r="C263" s="21"/>
@@ -8834,7 +8872,7 @@
       <c r="N263" s="8"/>
       <c r="O263" s="1"/>
     </row>
-    <row r="264" spans="1:15" ht="13.5" thickBot="1">
+    <row r="264" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A264" s="1"/>
       <c r="B264" s="21"/>
       <c r="C264" s="21"/>
@@ -8860,7 +8898,7 @@
       <c r="N264" s="8"/>
       <c r="O264" s="1"/>
     </row>
-    <row r="265" spans="1:15" ht="13.5" thickBot="1">
+    <row r="265" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A265" s="1"/>
       <c r="B265" s="21"/>
       <c r="C265" s="21"/>
@@ -8886,7 +8924,7 @@
       <c r="N265" s="8"/>
       <c r="O265" s="1"/>
     </row>
-    <row r="266" spans="1:15" ht="13.5" thickBot="1">
+    <row r="266" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A266" s="1"/>
       <c r="B266" s="21"/>
       <c r="C266" s="21"/>
@@ -8912,7 +8950,7 @@
       <c r="N266" s="8"/>
       <c r="O266" s="1"/>
     </row>
-    <row r="267" spans="1:15" ht="13.5" thickBot="1">
+    <row r="267" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A267" s="1"/>
       <c r="B267" s="21"/>
       <c r="C267" s="21"/>
@@ -8938,7 +8976,7 @@
       <c r="N267" s="8"/>
       <c r="O267" s="1"/>
     </row>
-    <row r="268" spans="1:15" ht="13.5" thickBot="1">
+    <row r="268" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A268" s="1"/>
       <c r="B268" s="21"/>
       <c r="C268" s="21"/>
@@ -8964,7 +9002,7 @@
       <c r="N268" s="8"/>
       <c r="O268" s="1"/>
     </row>
-    <row r="269" spans="1:15" ht="13.5" thickBot="1">
+    <row r="269" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A269" s="1"/>
       <c r="B269" s="21"/>
       <c r="C269" s="21"/>
@@ -8990,7 +9028,7 @@
       <c r="N269" s="8"/>
       <c r="O269" s="1"/>
     </row>
-    <row r="270" spans="1:15" ht="13.5" thickBot="1">
+    <row r="270" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A270" s="1"/>
       <c r="B270" s="21"/>
       <c r="C270" s="21"/>
@@ -9016,7 +9054,7 @@
       <c r="N270" s="8"/>
       <c r="O270" s="1"/>
     </row>
-    <row r="271" spans="1:15" ht="13.5" thickBot="1">
+    <row r="271" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A271" s="1"/>
       <c r="B271" s="21"/>
       <c r="C271" s="21"/>
@@ -9042,7 +9080,7 @@
       <c r="N271" s="8"/>
       <c r="O271" s="1"/>
     </row>
-    <row r="272" spans="1:15" ht="13.5" thickBot="1">
+    <row r="272" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A272" s="1"/>
       <c r="B272" s="21"/>
       <c r="C272" s="21"/>
@@ -9068,7 +9106,7 @@
       <c r="N272" s="8"/>
       <c r="O272" s="1"/>
     </row>
-    <row r="273" spans="1:15" ht="13.5" thickBot="1">
+    <row r="273" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A273" s="1"/>
       <c r="B273" s="21"/>
       <c r="C273" s="21"/>
@@ -9094,7 +9132,7 @@
       <c r="N273" s="8"/>
       <c r="O273" s="1"/>
     </row>
-    <row r="274" spans="1:15" ht="13.5" thickBot="1">
+    <row r="274" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A274" s="1"/>
       <c r="B274" s="21"/>
       <c r="C274" s="21"/>
@@ -9120,7 +9158,7 @@
       <c r="N274" s="8"/>
       <c r="O274" s="1"/>
     </row>
-    <row r="275" spans="1:15" ht="13.5" thickBot="1">
+    <row r="275" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A275" s="1"/>
       <c r="B275" s="21"/>
       <c r="C275" s="21"/>
@@ -9146,7 +9184,7 @@
       <c r="N275" s="8"/>
       <c r="O275" s="1"/>
     </row>
-    <row r="276" spans="1:15" ht="13.5" thickBot="1">
+    <row r="276" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A276" s="1"/>
       <c r="B276" s="21"/>
       <c r="C276" s="21"/>
@@ -9172,7 +9210,7 @@
       <c r="N276" s="8"/>
       <c r="O276" s="1"/>
     </row>
-    <row r="277" spans="1:15" ht="13.5" thickBot="1">
+    <row r="277" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A277" s="1"/>
       <c r="B277" s="21"/>
       <c r="C277" s="21"/>
@@ -9198,7 +9236,7 @@
       <c r="N277" s="8"/>
       <c r="O277" s="1"/>
     </row>
-    <row r="278" spans="1:15" ht="13.5" thickBot="1">
+    <row r="278" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A278" s="1"/>
       <c r="B278" s="21"/>
       <c r="C278" s="21"/>
@@ -9224,7 +9262,7 @@
       <c r="N278" s="8"/>
       <c r="O278" s="1"/>
     </row>
-    <row r="279" spans="1:15" ht="13.5" thickBot="1">
+    <row r="279" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A279" s="1"/>
       <c r="B279" s="21"/>
       <c r="C279" s="21"/>
@@ -9250,7 +9288,7 @@
       <c r="N279" s="8"/>
       <c r="O279" s="1"/>
     </row>
-    <row r="280" spans="1:15" ht="13.5" thickBot="1">
+    <row r="280" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A280" s="1"/>
       <c r="B280" s="21"/>
       <c r="C280" s="21"/>
@@ -9276,7 +9314,7 @@
       <c r="N280" s="8"/>
       <c r="O280" s="1"/>
     </row>
-    <row r="281" spans="1:15" ht="13.5" thickBot="1">
+    <row r="281" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A281" s="1"/>
       <c r="B281" s="21"/>
       <c r="C281" s="21"/>
@@ -9302,7 +9340,7 @@
       <c r="N281" s="8"/>
       <c r="O281" s="1"/>
     </row>
-    <row r="282" spans="1:15" ht="13.5" thickBot="1">
+    <row r="282" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A282" s="1"/>
       <c r="B282" s="21"/>
       <c r="C282" s="21"/>
@@ -9328,7 +9366,7 @@
       <c r="N282" s="8"/>
       <c r="O282" s="1"/>
     </row>
-    <row r="283" spans="1:15" ht="13.5" thickBot="1">
+    <row r="283" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A283" s="1"/>
       <c r="B283" s="21"/>
       <c r="C283" s="21"/>
@@ -9354,7 +9392,7 @@
       <c r="N283" s="8"/>
       <c r="O283" s="1"/>
     </row>
-    <row r="284" spans="1:15" ht="13.5" thickBot="1">
+    <row r="284" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A284" s="1"/>
       <c r="B284" s="21"/>
       <c r="C284" s="21"/>
@@ -9380,7 +9418,7 @@
       <c r="N284" s="8"/>
       <c r="O284" s="1"/>
     </row>
-    <row r="285" spans="1:15" ht="13.5" thickBot="1">
+    <row r="285" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A285" s="1"/>
       <c r="B285" s="21"/>
       <c r="C285" s="21"/>
@@ -9406,7 +9444,7 @@
       <c r="N285" s="8"/>
       <c r="O285" s="1"/>
     </row>
-    <row r="286" spans="1:15" ht="13.5" thickBot="1">
+    <row r="286" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A286" s="1"/>
       <c r="B286" s="21"/>
       <c r="C286" s="21"/>
@@ -9432,7 +9470,7 @@
       <c r="N286" s="8"/>
       <c r="O286" s="1"/>
     </row>
-    <row r="287" spans="1:15" ht="13.5" thickBot="1">
+    <row r="287" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A287" s="1"/>
       <c r="B287" s="21"/>
       <c r="C287" s="21"/>
@@ -9458,7 +9496,7 @@
       <c r="N287" s="8"/>
       <c r="O287" s="1"/>
     </row>
-    <row r="288" spans="1:15" ht="13.5" thickBot="1">
+    <row r="288" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A288" s="1"/>
       <c r="B288" s="21"/>
       <c r="C288" s="21"/>
@@ -9484,7 +9522,7 @@
       <c r="N288" s="8"/>
       <c r="O288" s="1"/>
     </row>
-    <row r="289" spans="1:15" ht="13.5" thickBot="1">
+    <row r="289" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A289" s="1"/>
       <c r="B289" s="21"/>
       <c r="C289" s="21"/>
@@ -9510,7 +9548,7 @@
       <c r="N289" s="8"/>
       <c r="O289" s="1"/>
     </row>
-    <row r="290" spans="1:15" ht="13.5" thickBot="1">
+    <row r="290" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A290" s="1"/>
       <c r="B290" s="21"/>
       <c r="C290" s="21"/>
@@ -9536,7 +9574,7 @@
       <c r="N290" s="8"/>
       <c r="O290" s="1"/>
     </row>
-    <row r="291" spans="1:15" ht="13.5" thickBot="1">
+    <row r="291" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A291" s="1"/>
       <c r="B291" s="21"/>
       <c r="C291" s="21"/>
@@ -9562,7 +9600,7 @@
       <c r="N291" s="8"/>
       <c r="O291" s="1"/>
     </row>
-    <row r="292" spans="1:15" ht="13.5" thickBot="1">
+    <row r="292" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A292" s="1"/>
       <c r="B292" s="21"/>
       <c r="C292" s="21"/>
@@ -9588,7 +9626,7 @@
       <c r="N292" s="8"/>
       <c r="O292" s="1"/>
     </row>
-    <row r="293" spans="1:15" ht="13.5" thickBot="1">
+    <row r="293" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A293" s="1"/>
       <c r="B293" s="21"/>
       <c r="C293" s="21"/>
@@ -9614,7 +9652,7 @@
       <c r="N293" s="8"/>
       <c r="O293" s="1"/>
     </row>
-    <row r="294" spans="1:15" ht="13.5" thickBot="1">
+    <row r="294" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A294" s="1"/>
       <c r="B294" s="21"/>
       <c r="C294" s="21"/>
@@ -9640,7 +9678,7 @@
       <c r="N294" s="8"/>
       <c r="O294" s="1"/>
     </row>
-    <row r="295" spans="1:15" ht="13.5" thickBot="1">
+    <row r="295" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A295" s="1"/>
       <c r="B295" s="21"/>
       <c r="C295" s="21"/>
@@ -9666,7 +9704,7 @@
       <c r="N295" s="8"/>
       <c r="O295" s="1"/>
     </row>
-    <row r="296" spans="1:15" ht="13.5" thickBot="1">
+    <row r="296" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A296" s="1"/>
       <c r="B296" s="21"/>
       <c r="C296" s="21"/>
@@ -9692,7 +9730,7 @@
       <c r="N296" s="8"/>
       <c r="O296" s="1"/>
     </row>
-    <row r="297" spans="1:15" ht="13.5" thickBot="1">
+    <row r="297" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A297" s="1"/>
       <c r="B297" s="21"/>
       <c r="C297" s="21"/>
@@ -9718,7 +9756,7 @@
       <c r="N297" s="8"/>
       <c r="O297" s="1"/>
     </row>
-    <row r="298" spans="1:15" ht="13.5" thickBot="1">
+    <row r="298" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A298" s="1"/>
       <c r="B298" s="21"/>
       <c r="C298" s="21"/>
@@ -9744,7 +9782,7 @@
       <c r="N298" s="8"/>
       <c r="O298" s="1"/>
     </row>
-    <row r="299" spans="1:15" ht="13.5" thickBot="1">
+    <row r="299" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A299" s="1"/>
       <c r="B299" s="21"/>
       <c r="C299" s="21"/>
@@ -9770,7 +9808,7 @@
       <c r="N299" s="8"/>
       <c r="O299" s="1"/>
     </row>
-    <row r="300" spans="1:15" ht="13.5" thickBot="1">
+    <row r="300" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A300" s="1"/>
       <c r="B300" s="21"/>
       <c r="C300" s="21"/>
@@ -9796,7 +9834,7 @@
       <c r="N300" s="8"/>
       <c r="O300" s="1"/>
     </row>
-    <row r="301" spans="1:15" ht="13.5" thickBot="1">
+    <row r="301" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A301" s="1"/>
       <c r="B301" s="21"/>
       <c r="C301" s="21"/>
@@ -9822,7 +9860,7 @@
       <c r="N301" s="8"/>
       <c r="O301" s="1"/>
     </row>
-    <row r="302" spans="1:15" ht="13.5" thickBot="1">
+    <row r="302" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A302" s="1"/>
       <c r="B302" s="21"/>
       <c r="C302" s="21"/>
@@ -9848,7 +9886,7 @@
       <c r="N302" s="8"/>
       <c r="O302" s="1"/>
     </row>
-    <row r="303" spans="1:15" ht="13.5" thickBot="1">
+    <row r="303" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A303" s="1"/>
       <c r="B303" s="21"/>
       <c r="C303" s="21"/>
@@ -9874,7 +9912,7 @@
       <c r="N303" s="8"/>
       <c r="O303" s="1"/>
     </row>
-    <row r="304" spans="1:15" ht="13.5" thickBot="1">
+    <row r="304" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A304" s="1"/>
       <c r="B304" s="21"/>
       <c r="C304" s="21"/>
@@ -9900,7 +9938,7 @@
       <c r="N304" s="8"/>
       <c r="O304" s="1"/>
     </row>
-    <row r="305" spans="1:15" ht="13.5" thickBot="1">
+    <row r="305" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A305" s="1"/>
       <c r="B305" s="21"/>
       <c r="C305" s="21"/>
@@ -9926,7 +9964,7 @@
       <c r="N305" s="8"/>
       <c r="O305" s="1"/>
     </row>
-    <row r="306" spans="1:15" ht="13.5" thickBot="1">
+    <row r="306" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A306" s="1"/>
       <c r="B306" s="21"/>
       <c r="C306" s="21"/>
@@ -9952,7 +9990,7 @@
       <c r="N306" s="8"/>
       <c r="O306" s="1"/>
     </row>
-    <row r="307" spans="1:15" ht="13.5" thickBot="1">
+    <row r="307" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A307" s="1"/>
       <c r="B307" s="21"/>
       <c r="C307" s="21"/>
@@ -9978,7 +10016,7 @@
       <c r="N307" s="8"/>
       <c r="O307" s="1"/>
     </row>
-    <row r="308" spans="1:15" ht="13.5" thickBot="1">
+    <row r="308" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A308" s="1"/>
       <c r="B308" s="21"/>
       <c r="C308" s="21"/>
@@ -10004,7 +10042,7 @@
       <c r="N308" s="8"/>
       <c r="O308" s="1"/>
     </row>
-    <row r="309" spans="1:15" ht="13.5" thickBot="1">
+    <row r="309" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A309" s="1"/>
       <c r="B309" s="21"/>
       <c r="C309" s="21"/>
@@ -10030,7 +10068,7 @@
       <c r="N309" s="8"/>
       <c r="O309" s="1"/>
     </row>
-    <row r="310" spans="1:15" ht="13.5" thickBot="1">
+    <row r="310" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A310" s="1"/>
       <c r="B310" s="21"/>
       <c r="C310" s="21"/>
@@ -10056,7 +10094,7 @@
       <c r="N310" s="8"/>
       <c r="O310" s="1"/>
     </row>
-    <row r="311" spans="1:15" ht="13.5" thickBot="1">
+    <row r="311" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A311" s="1"/>
       <c r="B311" s="21"/>
       <c r="C311" s="21"/>
@@ -10082,7 +10120,7 @@
       <c r="N311" s="8"/>
       <c r="O311" s="1"/>
     </row>
-    <row r="312" spans="1:15" ht="13.5" thickBot="1">
+    <row r="312" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A312" s="1"/>
       <c r="B312" s="21"/>
       <c r="C312" s="21"/>
@@ -10108,7 +10146,7 @@
       <c r="N312" s="8"/>
       <c r="O312" s="1"/>
     </row>
-    <row r="313" spans="1:15" ht="13.5" thickBot="1">
+    <row r="313" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A313" s="1"/>
       <c r="B313" s="21"/>
       <c r="C313" s="21"/>
@@ -10134,7 +10172,7 @@
       <c r="N313" s="8"/>
       <c r="O313" s="1"/>
     </row>
-    <row r="314" spans="1:15" ht="13.5" thickBot="1">
+    <row r="314" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A314" s="1"/>
       <c r="B314" s="21"/>
       <c r="C314" s="21"/>
@@ -10160,7 +10198,7 @@
       <c r="N314" s="8"/>
       <c r="O314" s="1"/>
     </row>
-    <row r="315" spans="1:15" ht="13.5" thickBot="1">
+    <row r="315" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A315" s="1"/>
       <c r="B315" s="21"/>
       <c r="C315" s="21"/>
@@ -10186,7 +10224,7 @@
       <c r="N315" s="8"/>
       <c r="O315" s="1"/>
     </row>
-    <row r="316" spans="1:15" ht="13.5" thickBot="1">
+    <row r="316" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A316" s="1"/>
       <c r="B316" s="21"/>
       <c r="C316" s="21"/>
@@ -10212,7 +10250,7 @@
       <c r="N316" s="8"/>
       <c r="O316" s="1"/>
     </row>
-    <row r="317" spans="1:15" ht="13.5" thickBot="1">
+    <row r="317" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A317" s="1"/>
       <c r="B317" s="21"/>
       <c r="C317" s="21"/>
@@ -10238,7 +10276,7 @@
       <c r="N317" s="8"/>
       <c r="O317" s="1"/>
     </row>
-    <row r="318" spans="1:15" ht="13.5" thickBot="1">
+    <row r="318" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A318" s="1"/>
       <c r="B318" s="21"/>
       <c r="C318" s="21"/>
@@ -10264,7 +10302,7 @@
       <c r="N318" s="8"/>
       <c r="O318" s="1"/>
     </row>
-    <row r="319" spans="1:15" ht="13.5" thickBot="1">
+    <row r="319" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A319" s="1"/>
       <c r="B319" s="21"/>
       <c r="C319" s="21"/>
@@ -10290,7 +10328,7 @@
       <c r="N319" s="8"/>
       <c r="O319" s="1"/>
     </row>
-    <row r="320" spans="1:15" ht="13.5" thickBot="1">
+    <row r="320" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A320" s="1"/>
       <c r="B320" s="21"/>
       <c r="C320" s="21"/>
@@ -10316,7 +10354,7 @@
       <c r="N320" s="8"/>
       <c r="O320" s="1"/>
     </row>
-    <row r="321" spans="1:15" ht="13.5" thickBot="1">
+    <row r="321" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A321" s="1"/>
       <c r="B321" s="21"/>
       <c r="C321" s="21"/>
@@ -10342,7 +10380,7 @@
       <c r="N321" s="8"/>
       <c r="O321" s="1"/>
     </row>
-    <row r="322" spans="1:15" ht="13.5" thickBot="1">
+    <row r="322" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A322" s="1"/>
       <c r="B322" s="21"/>
       <c r="C322" s="21"/>
@@ -10368,7 +10406,7 @@
       <c r="N322" s="8"/>
       <c r="O322" s="1"/>
     </row>
-    <row r="323" spans="1:15" ht="13.5" thickBot="1">
+    <row r="323" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A323" s="1"/>
       <c r="B323" s="21"/>
       <c r="C323" s="21"/>
@@ -10394,7 +10432,7 @@
       <c r="N323" s="8"/>
       <c r="O323" s="1"/>
     </row>
-    <row r="324" spans="1:15" ht="13.5" thickBot="1">
+    <row r="324" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A324" s="1"/>
       <c r="B324" s="21"/>
       <c r="C324" s="21"/>
@@ -10420,7 +10458,7 @@
       <c r="N324" s="8"/>
       <c r="O324" s="1"/>
     </row>
-    <row r="325" spans="1:15" ht="13.5" thickBot="1">
+    <row r="325" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A325" s="1"/>
       <c r="B325" s="21"/>
       <c r="C325" s="21"/>
@@ -10446,7 +10484,7 @@
       <c r="N325" s="8"/>
       <c r="O325" s="1"/>
     </row>
-    <row r="326" spans="1:15" ht="13.5" thickBot="1">
+    <row r="326" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A326" s="1"/>
       <c r="B326" s="21"/>
       <c r="C326" s="21"/>
@@ -10472,7 +10510,7 @@
       <c r="N326" s="8"/>
       <c r="O326" s="1"/>
     </row>
-    <row r="327" spans="1:15" ht="13.5" thickBot="1">
+    <row r="327" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A327" s="1"/>
       <c r="B327" s="21"/>
       <c r="C327" s="21"/>
@@ -10498,7 +10536,7 @@
       <c r="N327" s="8"/>
       <c r="O327" s="1"/>
     </row>
-    <row r="328" spans="1:15" ht="13.5" thickBot="1">
+    <row r="328" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A328" s="1"/>
       <c r="B328" s="21"/>
       <c r="C328" s="21"/>
@@ -10524,7 +10562,7 @@
       <c r="N328" s="8"/>
       <c r="O328" s="1"/>
     </row>
-    <row r="329" spans="1:15" ht="13.5" thickBot="1">
+    <row r="329" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A329" s="1"/>
       <c r="B329" s="21"/>
       <c r="C329" s="21"/>
@@ -10550,7 +10588,7 @@
       <c r="N329" s="8"/>
       <c r="O329" s="1"/>
     </row>
-    <row r="330" spans="1:15" ht="13.5" thickBot="1">
+    <row r="330" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A330" s="1"/>
       <c r="B330" s="21"/>
       <c r="C330" s="21"/>
@@ -10576,7 +10614,7 @@
       <c r="N330" s="8"/>
       <c r="O330" s="1"/>
     </row>
-    <row r="331" spans="1:15" ht="13.5" thickBot="1">
+    <row r="331" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A331" s="1"/>
       <c r="B331" s="21"/>
       <c r="C331" s="21"/>
@@ -10602,7 +10640,7 @@
       <c r="N331" s="8"/>
       <c r="O331" s="1"/>
     </row>
-    <row r="332" spans="1:15" ht="13.5" thickBot="1">
+    <row r="332" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A332" s="1"/>
       <c r="B332" s="21"/>
       <c r="C332" s="21"/>
@@ -10628,7 +10666,7 @@
       <c r="N332" s="8"/>
       <c r="O332" s="1"/>
     </row>
-    <row r="333" spans="1:15" ht="13.5" thickBot="1">
+    <row r="333" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A333" s="1"/>
       <c r="B333" s="21"/>
       <c r="C333" s="21"/>
@@ -10654,7 +10692,7 @@
       <c r="N333" s="8"/>
       <c r="O333" s="1"/>
     </row>
-    <row r="334" spans="1:15" ht="13.5" thickBot="1">
+    <row r="334" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A334" s="1"/>
       <c r="B334" s="21"/>
       <c r="C334" s="21"/>
@@ -10680,7 +10718,7 @@
       <c r="N334" s="8"/>
       <c r="O334" s="1"/>
     </row>
-    <row r="335" spans="1:15" ht="13.5" thickBot="1">
+    <row r="335" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A335" s="1"/>
       <c r="B335" s="21"/>
       <c r="C335" s="21"/>
@@ -10706,7 +10744,7 @@
       <c r="N335" s="8"/>
       <c r="O335" s="1"/>
     </row>
-    <row r="336" spans="1:15" ht="13.5" thickBot="1">
+    <row r="336" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A336" s="1"/>
       <c r="B336" s="21"/>
       <c r="C336" s="21"/>
@@ -10732,7 +10770,7 @@
       <c r="N336" s="8"/>
       <c r="O336" s="1"/>
     </row>
-    <row r="337" spans="1:15" ht="13.5" thickBot="1">
+    <row r="337" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A337" s="1"/>
       <c r="B337" s="21"/>
       <c r="C337" s="21"/>
@@ -10758,7 +10796,7 @@
       <c r="N337" s="8"/>
       <c r="O337" s="1"/>
     </row>
-    <row r="338" spans="1:15" ht="13.5" thickBot="1">
+    <row r="338" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A338" s="1"/>
       <c r="B338" s="21"/>
       <c r="C338" s="21"/>
@@ -10784,7 +10822,7 @@
       <c r="N338" s="8"/>
       <c r="O338" s="1"/>
     </row>
-    <row r="339" spans="1:15" ht="13.5" thickBot="1">
+    <row r="339" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A339" s="1"/>
       <c r="B339" s="21"/>
       <c r="C339" s="21"/>
@@ -10810,7 +10848,7 @@
       <c r="N339" s="8"/>
       <c r="O339" s="1"/>
     </row>
-    <row r="340" spans="1:15" ht="13.5" thickBot="1">
+    <row r="340" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A340" s="1"/>
       <c r="B340" s="21"/>
       <c r="C340" s="21"/>
@@ -10836,7 +10874,7 @@
       <c r="N340" s="8"/>
       <c r="O340" s="1"/>
     </row>
-    <row r="341" spans="1:15" ht="13.5" thickBot="1">
+    <row r="341" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A341" s="1"/>
       <c r="B341" s="21"/>
       <c r="C341" s="21"/>
@@ -10862,7 +10900,7 @@
       <c r="N341" s="8"/>
       <c r="O341" s="1"/>
     </row>
-    <row r="342" spans="1:15" ht="13.5" thickBot="1">
+    <row r="342" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A342" s="1"/>
       <c r="B342" s="21"/>
       <c r="C342" s="21"/>
@@ -10888,7 +10926,7 @@
       <c r="N342" s="8"/>
       <c r="O342" s="1"/>
     </row>
-    <row r="343" spans="1:15" ht="13.5" thickBot="1">
+    <row r="343" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A343" s="1"/>
       <c r="B343" s="21"/>
       <c r="C343" s="21"/>
@@ -10914,7 +10952,7 @@
       <c r="N343" s="8"/>
       <c r="O343" s="1"/>
     </row>
-    <row r="344" spans="1:15" ht="13.5" thickBot="1">
+    <row r="344" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A344" s="1"/>
       <c r="B344" s="21"/>
       <c r="C344" s="21"/>
@@ -10940,7 +10978,7 @@
       <c r="N344" s="8"/>
       <c r="O344" s="1"/>
     </row>
-    <row r="345" spans="1:15" ht="13.5" thickBot="1">
+    <row r="345" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A345" s="1"/>
       <c r="B345" s="21"/>
       <c r="C345" s="21"/>
@@ -10966,7 +11004,7 @@
       <c r="N345" s="8"/>
       <c r="O345" s="1"/>
     </row>
-    <row r="346" spans="1:15" ht="13.5" thickBot="1">
+    <row r="346" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A346" s="1"/>
       <c r="B346" s="21"/>
       <c r="C346" s="21"/>
@@ -10992,7 +11030,7 @@
       <c r="N346" s="8"/>
       <c r="O346" s="1"/>
     </row>
-    <row r="347" spans="1:15" ht="13.5" thickBot="1">
+    <row r="347" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A347" s="1"/>
       <c r="B347" s="21"/>
       <c r="C347" s="21"/>
@@ -11018,7 +11056,7 @@
       <c r="N347" s="8"/>
       <c r="O347" s="1"/>
     </row>
-    <row r="348" spans="1:15" ht="13.5" thickBot="1">
+    <row r="348" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A348" s="1"/>
       <c r="B348" s="21"/>
       <c r="C348" s="21"/>
@@ -11044,7 +11082,7 @@
       <c r="N348" s="8"/>
       <c r="O348" s="1"/>
     </row>
-    <row r="349" spans="1:15" ht="13.5" thickBot="1">
+    <row r="349" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A349" s="1"/>
       <c r="B349" s="21"/>
       <c r="C349" s="21"/>
@@ -11070,7 +11108,7 @@
       <c r="N349" s="8"/>
       <c r="O349" s="1"/>
     </row>
-    <row r="350" spans="1:15" ht="13.5" thickBot="1">
+    <row r="350" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A350" s="1"/>
       <c r="B350" s="21"/>
       <c r="C350" s="21"/>
@@ -11096,7 +11134,7 @@
       <c r="N350" s="8"/>
       <c r="O350" s="1"/>
     </row>
-    <row r="351" spans="1:15" ht="13.5" thickBot="1">
+    <row r="351" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A351" s="1"/>
       <c r="B351" s="21"/>
       <c r="C351" s="21"/>
@@ -11122,7 +11160,7 @@
       <c r="N351" s="8"/>
       <c r="O351" s="1"/>
     </row>
-    <row r="352" spans="1:15" ht="13.5" thickBot="1">
+    <row r="352" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A352" s="1"/>
       <c r="B352" s="21"/>
       <c r="C352" s="21"/>
@@ -11148,7 +11186,7 @@
       <c r="N352" s="8"/>
       <c r="O352" s="1"/>
     </row>
-    <row r="353" spans="1:15" ht="13.5" thickBot="1">
+    <row r="353" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A353" s="1"/>
       <c r="B353" s="21"/>
       <c r="C353" s="21"/>
@@ -11174,7 +11212,7 @@
       <c r="N353" s="8"/>
       <c r="O353" s="1"/>
     </row>
-    <row r="354" spans="1:15" ht="13.5" thickBot="1">
+    <row r="354" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A354" s="1"/>
       <c r="B354" s="21"/>
       <c r="C354" s="21"/>
@@ -11200,7 +11238,7 @@
       <c r="N354" s="8"/>
       <c r="O354" s="1"/>
     </row>
-    <row r="355" spans="1:15" ht="13.5" thickBot="1">
+    <row r="355" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A355" s="1"/>
       <c r="B355" s="21"/>
       <c r="C355" s="21"/>
@@ -11226,7 +11264,7 @@
       <c r="N355" s="8"/>
       <c r="O355" s="1"/>
     </row>
-    <row r="356" spans="1:15" ht="13.5" thickBot="1">
+    <row r="356" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A356" s="1"/>
       <c r="B356" s="21"/>
       <c r="C356" s="21"/>
@@ -11252,7 +11290,7 @@
       <c r="N356" s="8"/>
       <c r="O356" s="1"/>
     </row>
-    <row r="357" spans="1:15" ht="13.5" thickBot="1">
+    <row r="357" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A357" s="1"/>
       <c r="B357" s="21"/>
       <c r="C357" s="21"/>
@@ -11278,7 +11316,7 @@
       <c r="N357" s="8"/>
       <c r="O357" s="1"/>
     </row>
-    <row r="358" spans="1:15" ht="13.5" thickBot="1">
+    <row r="358" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A358" s="1"/>
       <c r="B358" s="21"/>
       <c r="C358" s="21"/>
@@ -11304,7 +11342,7 @@
       <c r="N358" s="8"/>
       <c r="O358" s="1"/>
     </row>
-    <row r="359" spans="1:15" ht="13.5" thickBot="1">
+    <row r="359" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A359" s="1"/>
       <c r="B359" s="21"/>
       <c r="C359" s="21"/>
@@ -11330,7 +11368,7 @@
       <c r="N359" s="8"/>
       <c r="O359" s="1"/>
     </row>
-    <row r="360" spans="1:15" ht="13.5" thickBot="1">
+    <row r="360" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A360" s="1"/>
       <c r="B360" s="21"/>
       <c r="C360" s="21"/>
@@ -11356,7 +11394,7 @@
       <c r="N360" s="8"/>
       <c r="O360" s="1"/>
     </row>
-    <row r="361" spans="1:15" ht="13.5" thickBot="1">
+    <row r="361" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A361" s="1"/>
       <c r="B361" s="21"/>
       <c r="C361" s="21"/>
@@ -11382,7 +11420,7 @@
       <c r="N361" s="8"/>
       <c r="O361" s="1"/>
     </row>
-    <row r="362" spans="1:15" ht="13.5" thickBot="1">
+    <row r="362" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A362" s="1"/>
       <c r="B362" s="21"/>
       <c r="C362" s="21"/>
@@ -11408,7 +11446,7 @@
       <c r="N362" s="8"/>
       <c r="O362" s="1"/>
     </row>
-    <row r="363" spans="1:15" ht="13.5" thickBot="1">
+    <row r="363" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A363" s="1"/>
       <c r="B363" s="21"/>
       <c r="C363" s="21"/>
@@ -11434,7 +11472,7 @@
       <c r="N363" s="8"/>
       <c r="O363" s="1"/>
     </row>
-    <row r="364" spans="1:15" ht="13.5" thickBot="1">
+    <row r="364" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A364" s="1"/>
       <c r="B364" s="21"/>
       <c r="C364" s="21"/>
@@ -11460,7 +11498,7 @@
       <c r="N364" s="8"/>
       <c r="O364" s="1"/>
     </row>
-    <row r="365" spans="1:15" ht="13.5" thickBot="1">
+    <row r="365" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A365" s="1"/>
       <c r="B365" s="21"/>
       <c r="C365" s="21"/>
@@ -11486,7 +11524,7 @@
       <c r="N365" s="8"/>
       <c r="O365" s="1"/>
     </row>
-    <row r="366" spans="1:15" ht="13.5" thickBot="1">
+    <row r="366" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A366" s="1"/>
       <c r="B366" s="21"/>
       <c r="C366" s="21"/>
@@ -11512,7 +11550,7 @@
       <c r="N366" s="8"/>
       <c r="O366" s="1"/>
     </row>
-    <row r="367" spans="1:15" ht="13.5" thickBot="1">
+    <row r="367" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A367" s="1"/>
       <c r="B367" s="21"/>
       <c r="C367" s="21"/>
@@ -11538,7 +11576,7 @@
       <c r="N367" s="8"/>
       <c r="O367" s="1"/>
     </row>
-    <row r="368" spans="1:15" ht="13.5" thickBot="1">
+    <row r="368" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A368" s="1"/>
       <c r="B368" s="21"/>
       <c r="C368" s="21"/>
@@ -11564,7 +11602,7 @@
       <c r="N368" s="8"/>
       <c r="O368" s="1"/>
     </row>
-    <row r="369" spans="1:15" ht="13.5" thickBot="1">
+    <row r="369" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A369" s="1"/>
       <c r="B369" s="21"/>
       <c r="C369" s="21"/>
@@ -11590,7 +11628,7 @@
       <c r="N369" s="8"/>
       <c r="O369" s="1"/>
     </row>
-    <row r="370" spans="1:15" ht="13.5" thickBot="1">
+    <row r="370" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A370" s="1"/>
       <c r="B370" s="21"/>
       <c r="C370" s="21"/>
@@ -11616,7 +11654,7 @@
       <c r="N370" s="8"/>
       <c r="O370" s="1"/>
     </row>
-    <row r="371" spans="1:15" ht="13.5" thickBot="1">
+    <row r="371" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A371" s="1"/>
       <c r="B371" s="21"/>
       <c r="C371" s="21"/>
@@ -11642,7 +11680,7 @@
       <c r="N371" s="8"/>
       <c r="O371" s="1"/>
     </row>
-    <row r="372" spans="1:15" ht="13.5" thickBot="1">
+    <row r="372" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A372" s="1"/>
       <c r="B372" s="21"/>
       <c r="C372" s="21"/>
@@ -11668,7 +11706,7 @@
       <c r="N372" s="8"/>
       <c r="O372" s="1"/>
     </row>
-    <row r="373" spans="1:15" ht="13.5" thickBot="1">
+    <row r="373" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A373" s="1"/>
       <c r="B373" s="21"/>
       <c r="C373" s="21"/>
@@ -11694,7 +11732,7 @@
       <c r="N373" s="8"/>
       <c r="O373" s="1"/>
     </row>
-    <row r="374" spans="1:15" ht="13.5" thickBot="1">
+    <row r="374" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A374" s="1"/>
       <c r="B374" s="21"/>
       <c r="C374" s="21"/>
@@ -11720,7 +11758,7 @@
       <c r="N374" s="8"/>
       <c r="O374" s="1"/>
     </row>
-    <row r="375" spans="1:15" ht="13.5" thickBot="1">
+    <row r="375" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A375" s="1"/>
       <c r="B375" s="21"/>
       <c r="C375" s="21"/>
@@ -11746,7 +11784,7 @@
       <c r="N375" s="8"/>
       <c r="O375" s="1"/>
     </row>
-    <row r="376" spans="1:15" ht="13.5" thickBot="1">
+    <row r="376" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A376" s="1"/>
       <c r="B376" s="21"/>
       <c r="C376" s="21"/>
@@ -11772,7 +11810,7 @@
       <c r="N376" s="8"/>
       <c r="O376" s="1"/>
     </row>
-    <row r="377" spans="1:15" ht="13.5" thickBot="1">
+    <row r="377" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A377" s="1"/>
       <c r="B377" s="21"/>
       <c r="C377" s="21"/>
@@ -11798,7 +11836,7 @@
       <c r="N377" s="8"/>
       <c r="O377" s="1"/>
     </row>
-    <row r="378" spans="1:15" ht="13.5" thickBot="1">
+    <row r="378" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A378" s="1"/>
       <c r="B378" s="21"/>
       <c r="C378" s="21"/>
@@ -11824,7 +11862,7 @@
       <c r="N378" s="8"/>
       <c r="O378" s="1"/>
     </row>
-    <row r="379" spans="1:15" ht="13.5" thickBot="1">
+    <row r="379" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A379" s="1"/>
       <c r="B379" s="21"/>
       <c r="C379" s="21"/>
@@ -11850,7 +11888,7 @@
       <c r="N379" s="8"/>
       <c r="O379" s="1"/>
     </row>
-    <row r="380" spans="1:15" ht="13.5" thickBot="1">
+    <row r="380" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A380" s="1"/>
       <c r="B380" s="21"/>
       <c r="C380" s="21"/>
@@ -11876,7 +11914,7 @@
       <c r="N380" s="8"/>
       <c r="O380" s="1"/>
     </row>
-    <row r="381" spans="1:15" ht="13.5" thickBot="1">
+    <row r="381" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A381" s="1"/>
       <c r="B381" s="21"/>
       <c r="C381" s="21"/>
@@ -11902,7 +11940,7 @@
       <c r="N381" s="8"/>
       <c r="O381" s="1"/>
     </row>
-    <row r="382" spans="1:15" ht="13.5" thickBot="1">
+    <row r="382" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A382" s="1"/>
       <c r="B382" s="21"/>
       <c r="C382" s="21"/>
@@ -11928,7 +11966,7 @@
       <c r="N382" s="8"/>
       <c r="O382" s="1"/>
     </row>
-    <row r="383" spans="1:15" ht="13.5" thickBot="1">
+    <row r="383" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A383" s="1"/>
       <c r="B383" s="21"/>
       <c r="C383" s="21"/>
@@ -11954,7 +11992,7 @@
       <c r="N383" s="8"/>
       <c r="O383" s="1"/>
     </row>
-    <row r="384" spans="1:15" ht="13.5" thickBot="1">
+    <row r="384" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A384" s="1"/>
       <c r="B384" s="21"/>
       <c r="C384" s="21"/>
@@ -11980,7 +12018,7 @@
       <c r="N384" s="8"/>
       <c r="O384" s="1"/>
     </row>
-    <row r="385" spans="1:15" ht="13.5" thickBot="1">
+    <row r="385" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A385" s="1"/>
       <c r="B385" s="21"/>
       <c r="C385" s="21"/>
@@ -12006,7 +12044,7 @@
       <c r="N385" s="8"/>
       <c r="O385" s="1"/>
     </row>
-    <row r="386" spans="1:15" ht="13.5" thickBot="1">
+    <row r="386" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A386" s="1"/>
       <c r="B386" s="21"/>
       <c r="C386" s="21"/>
@@ -12032,7 +12070,7 @@
       <c r="N386" s="8"/>
       <c r="O386" s="1"/>
     </row>
-    <row r="387" spans="1:15" ht="13.5" thickBot="1">
+    <row r="387" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A387" s="1"/>
       <c r="B387" s="21"/>
       <c r="C387" s="21"/>
@@ -12058,7 +12096,7 @@
       <c r="N387" s="8"/>
       <c r="O387" s="1"/>
     </row>
-    <row r="388" spans="1:15" ht="13.5" thickBot="1">
+    <row r="388" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A388" s="1"/>
       <c r="B388" s="21"/>
       <c r="C388" s="21"/>
@@ -12084,7 +12122,7 @@
       <c r="N388" s="8"/>
       <c r="O388" s="1"/>
     </row>
-    <row r="389" spans="1:15" ht="13.5" thickBot="1">
+    <row r="389" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A389" s="1"/>
       <c r="B389" s="21"/>
       <c r="C389" s="21"/>
@@ -12110,7 +12148,7 @@
       <c r="N389" s="8"/>
       <c r="O389" s="1"/>
     </row>
-    <row r="390" spans="1:15" ht="13.5" thickBot="1">
+    <row r="390" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A390" s="1"/>
       <c r="B390" s="21"/>
       <c r="C390" s="21"/>
@@ -12136,7 +12174,7 @@
       <c r="N390" s="8"/>
       <c r="O390" s="1"/>
     </row>
-    <row r="391" spans="1:15" ht="13.5" thickBot="1">
+    <row r="391" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A391" s="1"/>
       <c r="B391" s="21"/>
       <c r="C391" s="21"/>
@@ -12162,7 +12200,7 @@
       <c r="N391" s="8"/>
       <c r="O391" s="1"/>
     </row>
-    <row r="392" spans="1:15" ht="13.5" thickBot="1">
+    <row r="392" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A392" s="1"/>
       <c r="B392" s="21"/>
       <c r="C392" s="21"/>
@@ -12188,7 +12226,7 @@
       <c r="N392" s="8"/>
       <c r="O392" s="1"/>
     </row>
-    <row r="393" spans="1:15" ht="13.5" thickBot="1">
+    <row r="393" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A393" s="1"/>
       <c r="B393" s="21"/>
       <c r="C393" s="21"/>
@@ -12214,7 +12252,7 @@
       <c r="N393" s="8"/>
       <c r="O393" s="1"/>
     </row>
-    <row r="394" spans="1:15" ht="13.5" thickBot="1">
+    <row r="394" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A394" s="1"/>
       <c r="B394" s="21"/>
       <c r="C394" s="21"/>
@@ -12240,7 +12278,7 @@
       <c r="N394" s="8"/>
       <c r="O394" s="1"/>
     </row>
-    <row r="395" spans="1:15" ht="13.5" thickBot="1">
+    <row r="395" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A395" s="1"/>
       <c r="B395" s="21"/>
       <c r="C395" s="21"/>
@@ -12266,7 +12304,7 @@
       <c r="N395" s="8"/>
       <c r="O395" s="1"/>
     </row>
-    <row r="396" spans="1:15" ht="13.5" thickBot="1">
+    <row r="396" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A396" s="1"/>
       <c r="B396" s="21"/>
       <c r="C396" s="21"/>
@@ -12321,18 +12359,18 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="N6" r:id="rId1"/>
-    <hyperlink ref="N7" r:id="rId2"/>
-    <hyperlink ref="N9" r:id="rId3"/>
-    <hyperlink ref="N10" r:id="rId4"/>
-    <hyperlink ref="N11" r:id="rId5"/>
-    <hyperlink ref="N13" r:id="rId6"/>
-    <hyperlink ref="N14" r:id="rId7" location="gid=1874705319"/>
-    <hyperlink ref="N17" r:id="rId8"/>
-    <hyperlink ref="N18" r:id="rId9"/>
-    <hyperlink ref="N25" r:id="rId10"/>
-    <hyperlink ref="N26" r:id="rId11"/>
-    <hyperlink ref="N27" r:id="rId12"/>
+    <hyperlink ref="N6" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="N7" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="N9" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="N10" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="N11" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="N13" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="N14" r:id="rId7" location="gid=1874705319" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="N17" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="N18" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="N25" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="N26" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="N27" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
   </hyperlinks>
   <printOptions horizontalCentered="1" gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
@@ -12340,19 +12378,19 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" allowBlank="1">
+        <x14:dataValidation type="list" allowBlank="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
           <x14:formula1>
             <xm:f>'⚙️ Settings'!$D$2:$D$3</xm:f>
           </x14:formula1>
           <xm:sqref>M6:M30 M33:M396</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1">
+        <x14:dataValidation type="list" allowBlank="1" xr:uid="{00000000-0002-0000-0000-000001000000}">
           <x14:formula1>
             <xm:f>'⚙️ Settings'!$C$2:$C$10</xm:f>
           </x14:formula1>
           <xm:sqref>K6:K30 K33:K396</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1">
+        <x14:dataValidation type="list" allowBlank="1" xr:uid="{00000000-0002-0000-0000-000002000000}">
           <x14:formula1>
             <xm:f>'⚙️ Settings'!$E$2</xm:f>
           </x14:formula1>
@@ -12365,7 +12403,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor rgb="FF4A86E8"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -12376,7 +12414,7 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="0.85546875" style="21" customWidth="1"/>
     <col min="2" max="4" width="67.42578125" style="21" customWidth="1"/>
@@ -12384,14 +12422,14 @@
     <col min="6" max="16384" width="12.5703125" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="6" customHeight="1">
+    <row r="1" spans="1:5" ht="6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
     </row>
-    <row r="2" spans="1:5" ht="27" customHeight="1">
+    <row r="2" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="52" t="s">
         <v>65</v>
@@ -12400,14 +12438,14 @@
       <c r="D2" s="54"/>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:5" ht="27" customHeight="1">
+    <row r="3" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
       <c r="B3" s="55"/>
       <c r="C3" s="56"/>
       <c r="D3" s="57"/>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:5" ht="19.5" customHeight="1">
+    <row r="4" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
       <c r="B4" s="58" t="s">
         <v>1</v>
@@ -12420,14 +12458,14 @@
       </c>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="1:5" ht="19.5" customHeight="1">
+    <row r="5" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
       <c r="B5" s="46"/>
       <c r="C5" s="48"/>
       <c r="D5" s="44"/>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:5" ht="43.5" customHeight="1">
+    <row r="6" spans="1:5" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
       <c r="B6" s="25">
         <v>44691</v>
@@ -12440,14 +12478,14 @@
       </c>
       <c r="E6" s="1"/>
     </row>
-    <row r="7" spans="1:5" ht="43.5" customHeight="1">
+    <row r="7" spans="1:5" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
       <c r="B7" s="15"/>
       <c r="C7" s="15"/>
       <c r="D7" s="26"/>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:5" ht="43.5" customHeight="1">
+    <row r="8" spans="1:5" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
       <c r="B8" s="15"/>
       <c r="C8" s="15"/>
@@ -12466,7 +12504,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Information non valide">
+        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Information non valide" xr:uid="{00000000-0002-0000-0100-000000000000}">
           <x14:formula1>
             <xm:f>'⚙️ Settings'!$C$13:$C$15</xm:f>
           </x14:formula1>
@@ -12479,7 +12517,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor rgb="FF000000"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -12490,14 +12528,14 @@
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="25.42578125" customWidth="1"/>
     <col min="2" max="2" width="1.42578125" customWidth="1"/>
     <col min="3" max="26" width="25.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A1" s="16"/>
       <c r="B1" s="16"/>
       <c r="C1" s="17" t="s">
@@ -12531,7 +12569,7 @@
       <c r="Y1" s="16"/>
       <c r="Z1" s="16"/>
     </row>
-    <row r="2" spans="1:26">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A2" s="60" t="s">
         <v>50</v>
       </c>
@@ -12545,7 +12583,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:26">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A3" s="61"/>
       <c r="C3" s="19" t="s">
         <v>34</v>
@@ -12554,49 +12592,49 @@
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:26">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A4" s="61"/>
       <c r="C4" s="18" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:26">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A5" s="61"/>
       <c r="C5" s="18" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:26">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A6" s="61"/>
       <c r="C6" s="18" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:26">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A7" s="61"/>
       <c r="C7" s="18" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:26">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A8" s="61"/>
       <c r="C8" s="18" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:26">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A9" s="62"/>
       <c r="C9" s="18" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:26">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A10" s="20"/>
       <c r="C10" s="18" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:26">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A13" s="63" t="s">
         <v>72</v>
       </c>
@@ -12604,31 +12642,31 @@
         <v>73</v>
       </c>
     </row>
-    <row r="14" spans="1:26">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A14" s="61"/>
       <c r="C14" s="18" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="15" spans="1:26">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A15" s="61"/>
       <c r="C15" s="18" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="16" spans="1:26">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A16" s="61"/>
     </row>
-    <row r="17" spans="1:1">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" s="61"/>
     </row>
-    <row r="18" spans="1:1">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" s="61"/>
     </row>
-    <row r="19" spans="1:1">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" s="61"/>
     </row>
-    <row r="20" spans="1:1">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" s="62"/>
     </row>
   </sheetData>

</xml_diff>